<commit_message>
Debut de la creation des dispo
</commit_message>
<xml_diff>
--- a/Garde_V1.xlsx
+++ b/Garde_V1.xlsx
@@ -9,18 +9,19 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Administratif" sheetId="1" r:id="rId1"/>
     <sheet name="Import_GoogleForm" sheetId="2" r:id="rId2"/>
-    <sheet name="Weekend" sheetId="5" r:id="rId3"/>
-    <sheet name="Semaine" sheetId="6" r:id="rId4"/>
-    <sheet name="RecapSemaine" sheetId="4" r:id="rId5"/>
-    <sheet name="Stats" sheetId="3" r:id="rId6"/>
+    <sheet name="Besoins" sheetId="7" r:id="rId3"/>
+    <sheet name="Weekend" sheetId="5" r:id="rId4"/>
+    <sheet name="Semaine" sheetId="6" r:id="rId5"/>
+    <sheet name="RecapSemaine" sheetId="4" r:id="rId6"/>
+    <sheet name="Stats" sheetId="3" r:id="rId7"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId7"/>
+    <externalReference r:id="rId8"/>
   </externalReferences>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
@@ -30,15 +31,12 @@
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="700" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="751" uniqueCount="106">
   <si>
     <t>Noms</t>
   </si>
@@ -329,6 +327,33 @@
   </si>
   <si>
     <t>DISPONIBILITES</t>
+  </si>
+  <si>
+    <t>Vendredi</t>
+  </si>
+  <si>
+    <t>Nom</t>
+  </si>
+  <si>
+    <t>la semaine dernière</t>
+  </si>
+  <si>
+    <t>Nombre</t>
+  </si>
+  <si>
+    <t>d'astreinte</t>
+  </si>
+  <si>
+    <t>de garde</t>
+  </si>
+  <si>
+    <t>Disponibilité</t>
+  </si>
+  <si>
+    <t>Samedi</t>
+  </si>
+  <si>
+    <t>Dimanche</t>
   </si>
 </sst>
 </file>
@@ -1344,7 +1369,7 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="129">
+  <cellXfs count="132">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1565,19 +1590,68 @@
     <xf numFmtId="164" fontId="27" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="50" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="50" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="51" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="51" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="52" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="52" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="47" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="165" fontId="5" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="165" fontId="5" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="45" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="46" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="48" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="165" fontId="6" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1645,54 +1719,12 @@
     <xf numFmtId="0" fontId="11" fillId="4" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="45" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="46" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="47" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="48" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="50" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="50" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="51" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="51" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="52" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="52" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1700,7 +1732,7 @@
     <cellStyle name="Normal 2" xfId="2"/>
     <cellStyle name="Normal 4" xfId="1"/>
   </cellStyles>
-  <dxfs count="77">
+  <dxfs count="78">
     <dxf>
       <font>
         <color theme="0"/>
@@ -2562,14 +2594,21 @@
         </patternFill>
       </fill>
     </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -17122,8 +17161,8 @@
   <sheetPr codeName="Feuille2" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:AK53"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -17155,101 +17194,101 @@
       <c r="E3" s="82"/>
       <c r="F3" s="82"/>
       <c r="G3" s="82"/>
-      <c r="H3" s="92">
+      <c r="H3" s="109">
         <v>5</v>
       </c>
-      <c r="I3" s="92"/>
-      <c r="J3" s="92"/>
-      <c r="K3" s="92"/>
-      <c r="L3" s="93">
+      <c r="I3" s="109"/>
+      <c r="J3" s="109"/>
+      <c r="K3" s="109"/>
+      <c r="L3" s="110">
         <v>43129</v>
       </c>
-      <c r="M3" s="93"/>
-      <c r="N3" s="93"/>
-      <c r="O3" s="93"/>
-      <c r="P3" s="93"/>
-      <c r="Q3" s="93"/>
-      <c r="R3" s="93"/>
-      <c r="S3" s="94">
+      <c r="M3" s="110"/>
+      <c r="N3" s="110"/>
+      <c r="O3" s="110"/>
+      <c r="P3" s="110"/>
+      <c r="Q3" s="110"/>
+      <c r="R3" s="110"/>
+      <c r="S3" s="111">
         <f>L3+6</f>
         <v>43135</v>
       </c>
-      <c r="T3" s="94"/>
-      <c r="U3" s="94"/>
-      <c r="V3" s="94"/>
-      <c r="W3" s="94"/>
-      <c r="X3" s="94"/>
-      <c r="Y3" s="94"/>
-      <c r="Z3" s="94"/>
+      <c r="T3" s="111"/>
+      <c r="U3" s="111"/>
+      <c r="V3" s="111"/>
+      <c r="W3" s="111"/>
+      <c r="X3" s="111"/>
+      <c r="Y3" s="111"/>
+      <c r="Z3" s="111"/>
     </row>
     <row r="4" spans="1:37" ht="18" x14ac:dyDescent="0.2">
-      <c r="A4" s="84" t="s">
+      <c r="A4" s="97" t="s">
         <v>95</v>
       </c>
-      <c r="B4" s="117" t="s">
+      <c r="B4" s="103" t="s">
         <v>94</v>
       </c>
-      <c r="C4" s="87">
+      <c r="C4" s="100">
         <f>+$L$3</f>
         <v>43129</v>
       </c>
-      <c r="D4" s="87"/>
-      <c r="E4" s="87"/>
-      <c r="F4" s="87"/>
-      <c r="G4" s="88"/>
-      <c r="H4" s="86">
+      <c r="D4" s="100"/>
+      <c r="E4" s="100"/>
+      <c r="F4" s="100"/>
+      <c r="G4" s="101"/>
+      <c r="H4" s="102">
         <f>+C$4+1</f>
         <v>43130</v>
       </c>
-      <c r="I4" s="87"/>
-      <c r="J4" s="87"/>
-      <c r="K4" s="87"/>
-      <c r="L4" s="88"/>
-      <c r="M4" s="86">
-        <f t="shared" ref="M4" si="0">+H$4+1</f>
+      <c r="I4" s="100"/>
+      <c r="J4" s="100"/>
+      <c r="K4" s="100"/>
+      <c r="L4" s="101"/>
+      <c r="M4" s="102">
+        <f>+H$4+1</f>
         <v>43131</v>
       </c>
-      <c r="N4" s="87"/>
-      <c r="O4" s="87"/>
-      <c r="P4" s="87"/>
-      <c r="Q4" s="88"/>
-      <c r="R4" s="86">
-        <f t="shared" ref="R4" si="1">+M$4+1</f>
+      <c r="N4" s="100"/>
+      <c r="O4" s="100"/>
+      <c r="P4" s="100"/>
+      <c r="Q4" s="101"/>
+      <c r="R4" s="102">
+        <f>+M$4+1</f>
         <v>43132</v>
       </c>
-      <c r="S4" s="87"/>
-      <c r="T4" s="87"/>
-      <c r="U4" s="87"/>
-      <c r="V4" s="88"/>
-      <c r="W4" s="89">
+      <c r="S4" s="100"/>
+      <c r="T4" s="100"/>
+      <c r="U4" s="100"/>
+      <c r="V4" s="101"/>
+      <c r="W4" s="106">
         <f>+R$4+1</f>
         <v>43133</v>
       </c>
-      <c r="X4" s="90"/>
-      <c r="Y4" s="90"/>
-      <c r="Z4" s="90"/>
-      <c r="AA4" s="91"/>
-      <c r="AB4" s="89">
+      <c r="X4" s="107"/>
+      <c r="Y4" s="107"/>
+      <c r="Z4" s="107"/>
+      <c r="AA4" s="108"/>
+      <c r="AB4" s="106">
         <f>+W$4+1</f>
         <v>43134</v>
       </c>
-      <c r="AC4" s="90"/>
-      <c r="AD4" s="90"/>
-      <c r="AE4" s="90"/>
-      <c r="AF4" s="91"/>
-      <c r="AG4" s="89">
-        <f t="shared" ref="AG4" si="2">+AB$4+1</f>
+      <c r="AC4" s="107"/>
+      <c r="AD4" s="107"/>
+      <c r="AE4" s="107"/>
+      <c r="AF4" s="108"/>
+      <c r="AG4" s="106">
+        <f>+AB$4+1</f>
         <v>43135</v>
       </c>
-      <c r="AH4" s="90"/>
-      <c r="AI4" s="90"/>
-      <c r="AJ4" s="90"/>
-      <c r="AK4" s="91"/>
+      <c r="AH4" s="107"/>
+      <c r="AI4" s="107"/>
+      <c r="AJ4" s="107"/>
+      <c r="AK4" s="108"/>
     </row>
     <row r="5" spans="1:37" x14ac:dyDescent="0.2">
-      <c r="A5" s="85"/>
-      <c r="B5" s="118"/>
-      <c r="C5" s="115" t="s">
+      <c r="A5" s="98"/>
+      <c r="B5" s="104"/>
+      <c r="C5" s="87" t="s">
         <v>51</v>
       </c>
       <c r="D5" s="10" t="s">
@@ -17356,9 +17395,9 @@
       </c>
     </row>
     <row r="6" spans="1:37" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="119"/>
-      <c r="B6" s="120"/>
-      <c r="C6" s="116" t="s">
+      <c r="A6" s="99"/>
+      <c r="B6" s="105"/>
+      <c r="C6" s="88" t="s">
         <v>52</v>
       </c>
       <c r="D6" s="13" t="s">
@@ -17465,14 +17504,14 @@
       </c>
     </row>
     <row r="7" spans="1:37" x14ac:dyDescent="0.2">
-      <c r="A7" s="123">
+      <c r="A7" s="91">
         <f>VLOOKUP(Import_GoogleForm!$B7,Administratif!$A$3:$C$100,3,FALSE)</f>
         <v>2</v>
       </c>
-      <c r="B7" s="124" t="s">
+      <c r="B7" s="92" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="121"/>
+      <c r="C7" s="89"/>
       <c r="D7" s="3"/>
       <c r="E7" s="3" t="s">
         <v>42</v>
@@ -17525,14 +17564,14 @@
       <c r="AK7" s="4"/>
     </row>
     <row r="8" spans="1:37" x14ac:dyDescent="0.2">
-      <c r="A8" s="125">
+      <c r="A8" s="93">
         <f>VLOOKUP(Import_GoogleForm!$B8,Administratif!$A$3:$C$100,3,FALSE)</f>
         <v>1</v>
       </c>
-      <c r="B8" s="126" t="s">
+      <c r="B8" s="94" t="s">
         <v>21</v>
       </c>
-      <c r="C8" s="122" t="s">
+      <c r="C8" s="90" t="s">
         <v>42</v>
       </c>
       <c r="D8" s="5" t="s">
@@ -17597,14 +17636,14 @@
       <c r="AK8" s="6"/>
     </row>
     <row r="9" spans="1:37" x14ac:dyDescent="0.2">
-      <c r="A9" s="125">
+      <c r="A9" s="93">
         <f>VLOOKUP(Import_GoogleForm!$B9,Administratif!$A$3:$C$100,3,FALSE)</f>
         <v>3</v>
       </c>
-      <c r="B9" s="126" t="s">
+      <c r="B9" s="94" t="s">
         <v>13</v>
       </c>
-      <c r="C9" s="122"/>
+      <c r="C9" s="90"/>
       <c r="D9" s="5"/>
       <c r="E9" s="5"/>
       <c r="F9" s="5" t="s">
@@ -17647,14 +17686,14 @@
       <c r="AK9" s="6"/>
     </row>
     <row r="10" spans="1:37" x14ac:dyDescent="0.2">
-      <c r="A10" s="125">
+      <c r="A10" s="93">
         <f>VLOOKUP(Import_GoogleForm!$B10,Administratif!$A$3:$C$100,3,FALSE)</f>
         <v>4</v>
       </c>
-      <c r="B10" s="126" t="s">
+      <c r="B10" s="94" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="122"/>
+      <c r="C10" s="90"/>
       <c r="D10" s="5"/>
       <c r="E10" s="5"/>
       <c r="F10" s="5" t="s">
@@ -17707,14 +17746,14 @@
       <c r="AK10" s="6"/>
     </row>
     <row r="11" spans="1:37" x14ac:dyDescent="0.2">
-      <c r="A11" s="125">
+      <c r="A11" s="93">
         <f>VLOOKUP(Import_GoogleForm!$B11,Administratif!$A$3:$C$100,3,FALSE)</f>
         <v>2</v>
       </c>
-      <c r="B11" s="126" t="s">
+      <c r="B11" s="94" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="122" t="s">
+      <c r="C11" s="90" t="s">
         <v>43</v>
       </c>
       <c r="D11" s="5" t="s">
@@ -17821,14 +17860,14 @@
       </c>
     </row>
     <row r="12" spans="1:37" x14ac:dyDescent="0.2">
-      <c r="A12" s="125">
+      <c r="A12" s="93">
         <f>VLOOKUP(Import_GoogleForm!$B12,Administratif!$A$3:$C$100,3,FALSE)</f>
         <v>2</v>
       </c>
-      <c r="B12" s="126" t="s">
+      <c r="B12" s="94" t="s">
         <v>14</v>
       </c>
-      <c r="C12" s="122"/>
+      <c r="C12" s="90"/>
       <c r="D12" s="5" t="s">
         <v>42</v>
       </c>
@@ -17887,14 +17926,14 @@
       <c r="AK12" s="6"/>
     </row>
     <row r="13" spans="1:37" x14ac:dyDescent="0.2">
-      <c r="A13" s="125">
+      <c r="A13" s="93">
         <f>VLOOKUP(Import_GoogleForm!$B13,Administratif!$A$3:$C$100,3,FALSE)</f>
         <v>1</v>
       </c>
-      <c r="B13" s="126" t="s">
+      <c r="B13" s="94" t="s">
         <v>7</v>
       </c>
-      <c r="C13" s="122"/>
+      <c r="C13" s="90"/>
       <c r="D13" s="5"/>
       <c r="E13" s="5"/>
       <c r="F13" s="5"/>
@@ -17943,14 +17982,14 @@
       <c r="AK13" s="6"/>
     </row>
     <row r="14" spans="1:37" x14ac:dyDescent="0.2">
-      <c r="A14" s="125">
+      <c r="A14" s="93">
         <f>VLOOKUP(Import_GoogleForm!$B14,Administratif!$A$3:$C$100,3,FALSE)</f>
         <v>2</v>
       </c>
-      <c r="B14" s="126" t="s">
+      <c r="B14" s="94" t="s">
         <v>44</v>
       </c>
-      <c r="C14" s="122"/>
+      <c r="C14" s="90"/>
       <c r="D14" s="5"/>
       <c r="E14" s="5"/>
       <c r="F14" s="5"/>
@@ -17991,14 +18030,14 @@
       <c r="AK14" s="6"/>
     </row>
     <row r="15" spans="1:37" x14ac:dyDescent="0.2">
-      <c r="A15" s="125">
+      <c r="A15" s="93">
         <f>VLOOKUP(Import_GoogleForm!$B15,Administratif!$A$3:$C$100,3,FALSE)</f>
         <v>3</v>
       </c>
-      <c r="B15" s="126" t="s">
+      <c r="B15" s="94" t="s">
         <v>45</v>
       </c>
-      <c r="C15" s="122" t="s">
+      <c r="C15" s="90" t="s">
         <v>43</v>
       </c>
       <c r="D15" s="5" t="s">
@@ -18105,14 +18144,14 @@
       </c>
     </row>
     <row r="16" spans="1:37" x14ac:dyDescent="0.2">
-      <c r="A16" s="125">
+      <c r="A16" s="93">
         <f>VLOOKUP(Import_GoogleForm!$B16,Administratif!$A$3:$C$100,3,FALSE)</f>
         <v>4</v>
       </c>
-      <c r="B16" s="126" t="s">
+      <c r="B16" s="94" t="s">
         <v>46</v>
       </c>
-      <c r="C16" s="122"/>
+      <c r="C16" s="90"/>
       <c r="D16" s="5"/>
       <c r="E16" s="5"/>
       <c r="F16" s="5"/>
@@ -18155,14 +18194,14 @@
       <c r="AK16" s="6"/>
     </row>
     <row r="17" spans="1:37" x14ac:dyDescent="0.2">
-      <c r="A17" s="125">
+      <c r="A17" s="93">
         <f>VLOOKUP(Import_GoogleForm!$B17,Administratif!$A$3:$C$100,3,FALSE)</f>
         <v>1</v>
       </c>
-      <c r="B17" s="126" t="s">
+      <c r="B17" s="94" t="s">
         <v>47</v>
       </c>
-      <c r="C17" s="122"/>
+      <c r="C17" s="90"/>
       <c r="D17" s="5"/>
       <c r="E17" s="5"/>
       <c r="F17" s="5"/>
@@ -18217,14 +18256,14 @@
       <c r="AK17" s="6"/>
     </row>
     <row r="18" spans="1:37" x14ac:dyDescent="0.2">
-      <c r="A18" s="125">
+      <c r="A18" s="93">
         <f>VLOOKUP(Import_GoogleForm!$B18,Administratif!$A$3:$C$100,3,FALSE)</f>
         <v>2</v>
       </c>
-      <c r="B18" s="126" t="s">
+      <c r="B18" s="94" t="s">
         <v>16</v>
       </c>
-      <c r="C18" s="122" t="s">
+      <c r="C18" s="90" t="s">
         <v>42</v>
       </c>
       <c r="D18" s="5" t="s">
@@ -18317,14 +18356,14 @@
       </c>
     </row>
     <row r="19" spans="1:37" x14ac:dyDescent="0.2">
-      <c r="A19" s="125">
+      <c r="A19" s="93">
         <f>VLOOKUP(Import_GoogleForm!$B19,Administratif!$A$3:$C$100,3,FALSE)</f>
         <v>4</v>
       </c>
-      <c r="B19" s="126" t="s">
+      <c r="B19" s="94" t="s">
         <v>25</v>
       </c>
-      <c r="C19" s="122"/>
+      <c r="C19" s="90"/>
       <c r="D19" s="5"/>
       <c r="E19" s="5"/>
       <c r="F19" s="5"/>
@@ -18365,14 +18404,14 @@
       <c r="AK19" s="6"/>
     </row>
     <row r="20" spans="1:37" x14ac:dyDescent="0.2">
-      <c r="A20" s="125">
+      <c r="A20" s="93">
         <f>VLOOKUP(Import_GoogleForm!$B20,Administratif!$A$3:$C$100,3,FALSE)</f>
         <v>1</v>
       </c>
-      <c r="B20" s="126" t="s">
+      <c r="B20" s="94" t="s">
         <v>24</v>
       </c>
-      <c r="C20" s="122"/>
+      <c r="C20" s="90"/>
       <c r="D20" s="5"/>
       <c r="E20" s="5"/>
       <c r="F20" s="5"/>
@@ -18413,14 +18452,14 @@
       <c r="AK20" s="6"/>
     </row>
     <row r="21" spans="1:37" x14ac:dyDescent="0.2">
-      <c r="A21" s="125">
+      <c r="A21" s="93">
         <f>VLOOKUP(Import_GoogleForm!$B21,Administratif!$A$3:$C$100,3,FALSE)</f>
         <v>4</v>
       </c>
-      <c r="B21" s="126" t="s">
+      <c r="B21" s="94" t="s">
         <v>28</v>
       </c>
-      <c r="C21" s="122"/>
+      <c r="C21" s="90"/>
       <c r="D21" s="5" t="s">
         <v>42</v>
       </c>
@@ -18481,14 +18520,14 @@
       <c r="AK21" s="6"/>
     </row>
     <row r="22" spans="1:37" x14ac:dyDescent="0.2">
-      <c r="A22" s="125">
+      <c r="A22" s="93">
         <f>VLOOKUP(Import_GoogleForm!$B22,Administratif!$A$3:$C$100,3,FALSE)</f>
         <v>3</v>
       </c>
-      <c r="B22" s="126" t="s">
+      <c r="B22" s="94" t="s">
         <v>6</v>
       </c>
-      <c r="C22" s="122"/>
+      <c r="C22" s="90"/>
       <c r="D22" s="5"/>
       <c r="E22" s="5"/>
       <c r="F22" s="5"/>
@@ -18527,14 +18566,14 @@
       <c r="AK22" s="6"/>
     </row>
     <row r="23" spans="1:37" x14ac:dyDescent="0.2">
-      <c r="A23" s="125">
+      <c r="A23" s="93">
         <f>VLOOKUP(Import_GoogleForm!$B23,Administratif!$A$3:$C$100,3,FALSE)</f>
         <v>2</v>
       </c>
-      <c r="B23" s="126" t="s">
+      <c r="B23" s="94" t="s">
         <v>8</v>
       </c>
-      <c r="C23" s="122" t="s">
+      <c r="C23" s="90" t="s">
         <v>42</v>
       </c>
       <c r="D23" s="5" t="s">
@@ -18621,14 +18660,14 @@
       </c>
     </row>
     <row r="24" spans="1:37" x14ac:dyDescent="0.2">
-      <c r="A24" s="125">
+      <c r="A24" s="93">
         <f>VLOOKUP(Import_GoogleForm!$B24,Administratif!$A$3:$C$100,3,FALSE)</f>
         <v>2</v>
       </c>
-      <c r="B24" s="126" t="s">
+      <c r="B24" s="94" t="s">
         <v>48</v>
       </c>
-      <c r="C24" s="122"/>
+      <c r="C24" s="90"/>
       <c r="D24" s="5"/>
       <c r="E24" s="5"/>
       <c r="F24" s="5"/>
@@ -18677,14 +18716,14 @@
       <c r="AK24" s="6"/>
     </row>
     <row r="25" spans="1:37" x14ac:dyDescent="0.2">
-      <c r="A25" s="125">
+      <c r="A25" s="93">
         <f>VLOOKUP(Import_GoogleForm!$B25,Administratif!$A$3:$C$100,3,FALSE)</f>
         <v>4</v>
       </c>
-      <c r="B25" s="126" t="s">
+      <c r="B25" s="94" t="s">
         <v>20</v>
       </c>
-      <c r="C25" s="122"/>
+      <c r="C25" s="90"/>
       <c r="D25" s="5"/>
       <c r="E25" s="5"/>
       <c r="F25" s="5"/>
@@ -18725,14 +18764,14 @@
       <c r="AK25" s="6"/>
     </row>
     <row r="26" spans="1:37" x14ac:dyDescent="0.2">
-      <c r="A26" s="125">
+      <c r="A26" s="93">
         <f>VLOOKUP(Import_GoogleForm!$B26,Administratif!$A$3:$C$100,3,FALSE)</f>
         <v>3</v>
       </c>
-      <c r="B26" s="126" t="s">
+      <c r="B26" s="94" t="s">
         <v>49</v>
       </c>
-      <c r="C26" s="122"/>
+      <c r="C26" s="90"/>
       <c r="D26" s="5"/>
       <c r="E26" s="5"/>
       <c r="F26" s="5"/>
@@ -18771,14 +18810,14 @@
       <c r="AK26" s="6"/>
     </row>
     <row r="27" spans="1:37" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="127">
+      <c r="A27" s="95">
         <f>VLOOKUP(Import_GoogleForm!$B27,Administratif!$A$3:$C$100,3,FALSE)</f>
         <v>4</v>
       </c>
-      <c r="B27" s="128" t="s">
+      <c r="B27" s="96" t="s">
         <v>22</v>
       </c>
-      <c r="C27" s="122"/>
+      <c r="C27" s="90"/>
       <c r="D27" s="5" t="s">
         <v>42</v>
       </c>
@@ -18819,76 +18858,76 @@
       <c r="AK27" s="6"/>
     </row>
     <row r="30" spans="1:37" x14ac:dyDescent="0.2">
-      <c r="B30" s="114"/>
+      <c r="B30" s="86"/>
     </row>
     <row r="31" spans="1:37" x14ac:dyDescent="0.2">
-      <c r="B31" s="114"/>
+      <c r="B31" s="86"/>
     </row>
     <row r="32" spans="1:37" x14ac:dyDescent="0.2">
-      <c r="B32" s="114"/>
+      <c r="B32" s="86"/>
     </row>
     <row r="33" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B33" s="112"/>
+      <c r="B33" s="84"/>
     </row>
     <row r="34" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B34" s="113"/>
+      <c r="B34" s="85"/>
     </row>
     <row r="35" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B35" s="113"/>
+      <c r="B35" s="85"/>
     </row>
     <row r="36" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B36" s="113"/>
+      <c r="B36" s="85"/>
     </row>
     <row r="37" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B37" s="113"/>
+      <c r="B37" s="85"/>
     </row>
     <row r="38" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B38" s="113"/>
+      <c r="B38" s="85"/>
     </row>
     <row r="39" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B39" s="113"/>
+      <c r="B39" s="85"/>
     </row>
     <row r="40" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B40" s="113"/>
+      <c r="B40" s="85"/>
     </row>
     <row r="41" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B41" s="113"/>
+      <c r="B41" s="85"/>
     </row>
     <row r="42" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B42" s="113"/>
+      <c r="B42" s="85"/>
     </row>
     <row r="43" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B43" s="113"/>
+      <c r="B43" s="85"/>
     </row>
     <row r="44" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B44" s="113"/>
+      <c r="B44" s="85"/>
     </row>
     <row r="45" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B45" s="113"/>
+      <c r="B45" s="85"/>
     </row>
     <row r="46" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B46" s="113"/>
+      <c r="B46" s="85"/>
     </row>
     <row r="47" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B47" s="113"/>
+      <c r="B47" s="85"/>
     </row>
     <row r="48" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B48" s="113"/>
+      <c r="B48" s="85"/>
     </row>
     <row r="49" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B49" s="113"/>
+      <c r="B49" s="85"/>
     </row>
     <row r="50" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B50" s="113"/>
+      <c r="B50" s="85"/>
     </row>
     <row r="51" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B51" s="113"/>
+      <c r="B51" s="85"/>
     </row>
     <row r="52" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B52" s="113"/>
+      <c r="B52" s="85"/>
     </row>
     <row r="53" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B53" s="113"/>
+      <c r="B53" s="85"/>
     </row>
   </sheetData>
   <mergeCells count="12">
@@ -18911,6 +18950,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Feuille3" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -18923,6 +18963,849 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Feuille4" enableFormatConditionsCalculation="0"/>
+  <dimension ref="B16:AA42"/>
+  <sheetViews>
+    <sheetView topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="T16" sqref="T16:AA16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="21.6640625" customWidth="1"/>
+    <col min="11" max="11" width="21.6640625" customWidth="1"/>
+    <col min="20" max="20" width="21.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="16" spans="2:27" x14ac:dyDescent="0.2">
+      <c r="B16" s="130" t="s">
+        <v>97</v>
+      </c>
+      <c r="C16" s="130"/>
+      <c r="D16" s="130"/>
+      <c r="E16" s="130"/>
+      <c r="F16" s="130"/>
+      <c r="G16" s="130"/>
+      <c r="H16" s="130"/>
+      <c r="I16" s="130"/>
+      <c r="K16" s="130" t="s">
+        <v>104</v>
+      </c>
+      <c r="L16" s="130"/>
+      <c r="M16" s="130"/>
+      <c r="N16" s="130"/>
+      <c r="O16" s="130"/>
+      <c r="P16" s="130"/>
+      <c r="Q16" s="130"/>
+      <c r="R16" s="130"/>
+      <c r="T16" s="130" t="s">
+        <v>105</v>
+      </c>
+      <c r="U16" s="130"/>
+      <c r="V16" s="130"/>
+      <c r="W16" s="130"/>
+      <c r="X16" s="130"/>
+      <c r="Y16" s="130"/>
+      <c r="Z16" s="130"/>
+      <c r="AA16" s="130"/>
+    </row>
+    <row r="17" spans="2:27" x14ac:dyDescent="0.2">
+      <c r="B17" s="130" t="s">
+        <v>98</v>
+      </c>
+      <c r="C17" s="130" t="s">
+        <v>100</v>
+      </c>
+      <c r="D17" s="130"/>
+      <c r="E17" s="130" t="s">
+        <v>103</v>
+      </c>
+      <c r="F17" s="130"/>
+      <c r="G17" s="130"/>
+      <c r="H17" s="130"/>
+      <c r="I17" s="130"/>
+      <c r="K17" s="130" t="s">
+        <v>98</v>
+      </c>
+      <c r="L17" s="130" t="s">
+        <v>100</v>
+      </c>
+      <c r="M17" s="130"/>
+      <c r="N17" s="130" t="s">
+        <v>103</v>
+      </c>
+      <c r="O17" s="130"/>
+      <c r="P17" s="130"/>
+      <c r="Q17" s="130"/>
+      <c r="R17" s="130"/>
+      <c r="T17" s="130" t="s">
+        <v>98</v>
+      </c>
+      <c r="U17" s="130" t="s">
+        <v>100</v>
+      </c>
+      <c r="V17" s="130"/>
+      <c r="W17" s="130" t="s">
+        <v>103</v>
+      </c>
+      <c r="X17" s="130"/>
+      <c r="Y17" s="130"/>
+      <c r="Z17" s="130"/>
+      <c r="AA17" s="130"/>
+    </row>
+    <row r="18" spans="2:27" x14ac:dyDescent="0.2">
+      <c r="B18" s="130"/>
+      <c r="C18" s="131" t="s">
+        <v>102</v>
+      </c>
+      <c r="D18" s="131" t="s">
+        <v>101</v>
+      </c>
+      <c r="E18" s="131" t="s">
+        <v>51</v>
+      </c>
+      <c r="F18" s="131" t="s">
+        <v>52</v>
+      </c>
+      <c r="G18" s="131" t="s">
+        <v>53</v>
+      </c>
+      <c r="H18" s="131" t="s">
+        <v>54</v>
+      </c>
+      <c r="I18" s="131" t="s">
+        <v>55</v>
+      </c>
+      <c r="K18" s="130"/>
+      <c r="L18" s="131" t="s">
+        <v>102</v>
+      </c>
+      <c r="M18" s="131" t="s">
+        <v>101</v>
+      </c>
+      <c r="N18" s="131" t="s">
+        <v>51</v>
+      </c>
+      <c r="O18" s="131" t="s">
+        <v>52</v>
+      </c>
+      <c r="P18" s="131" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q18" s="131" t="s">
+        <v>54</v>
+      </c>
+      <c r="R18" s="131" t="s">
+        <v>55</v>
+      </c>
+      <c r="T18" s="130"/>
+      <c r="U18" s="131" t="s">
+        <v>102</v>
+      </c>
+      <c r="V18" s="131" t="s">
+        <v>101</v>
+      </c>
+      <c r="W18" s="131" t="s">
+        <v>51</v>
+      </c>
+      <c r="X18" s="131" t="s">
+        <v>52</v>
+      </c>
+      <c r="Y18" s="131" t="s">
+        <v>53</v>
+      </c>
+      <c r="Z18" s="131" t="s">
+        <v>54</v>
+      </c>
+      <c r="AA18" s="131" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="19" spans="2:27" x14ac:dyDescent="0.2">
+      <c r="B19" s="130"/>
+      <c r="C19" s="130" t="s">
+        <v>99</v>
+      </c>
+      <c r="D19" s="130"/>
+      <c r="E19" s="131" t="s">
+        <v>52</v>
+      </c>
+      <c r="F19" s="131" t="s">
+        <v>53</v>
+      </c>
+      <c r="G19" s="131" t="s">
+        <v>54</v>
+      </c>
+      <c r="H19" s="131" t="s">
+        <v>55</v>
+      </c>
+      <c r="I19" s="131" t="s">
+        <v>51</v>
+      </c>
+      <c r="K19" s="130"/>
+      <c r="L19" s="130" t="s">
+        <v>99</v>
+      </c>
+      <c r="M19" s="130"/>
+      <c r="N19" s="131" t="s">
+        <v>52</v>
+      </c>
+      <c r="O19" s="131" t="s">
+        <v>53</v>
+      </c>
+      <c r="P19" s="131" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q19" s="131" t="s">
+        <v>55</v>
+      </c>
+      <c r="R19" s="131" t="s">
+        <v>51</v>
+      </c>
+      <c r="T19" s="130"/>
+      <c r="U19" s="130" t="s">
+        <v>99</v>
+      </c>
+      <c r="V19" s="130"/>
+      <c r="W19" s="131" t="s">
+        <v>52</v>
+      </c>
+      <c r="X19" s="131" t="s">
+        <v>53</v>
+      </c>
+      <c r="Y19" s="131" t="s">
+        <v>54</v>
+      </c>
+      <c r="Z19" s="131" t="s">
+        <v>55</v>
+      </c>
+      <c r="AA19" s="131" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="20" spans="2:27" x14ac:dyDescent="0.2">
+      <c r="B20" s="129"/>
+      <c r="C20" s="129"/>
+      <c r="D20" s="129"/>
+      <c r="E20" s="129"/>
+      <c r="F20" s="129"/>
+      <c r="G20" s="129"/>
+      <c r="H20" s="129"/>
+      <c r="I20" s="129"/>
+      <c r="K20" s="129"/>
+      <c r="L20" s="129"/>
+      <c r="M20" s="129"/>
+      <c r="N20" s="129"/>
+      <c r="O20" s="129"/>
+      <c r="P20" s="129"/>
+      <c r="Q20" s="129"/>
+      <c r="R20" s="129"/>
+      <c r="T20" s="129"/>
+      <c r="U20" s="129"/>
+      <c r="V20" s="129"/>
+      <c r="W20" s="129"/>
+      <c r="X20" s="129"/>
+      <c r="Y20" s="129"/>
+      <c r="Z20" s="129"/>
+      <c r="AA20" s="129"/>
+    </row>
+    <row r="21" spans="2:27" x14ac:dyDescent="0.2">
+      <c r="B21" s="129"/>
+      <c r="C21" s="129"/>
+      <c r="D21" s="129"/>
+      <c r="E21" s="129"/>
+      <c r="F21" s="129"/>
+      <c r="G21" s="129"/>
+      <c r="H21" s="129"/>
+      <c r="I21" s="129"/>
+      <c r="K21" s="129"/>
+      <c r="L21" s="129"/>
+      <c r="M21" s="129"/>
+      <c r="N21" s="129"/>
+      <c r="O21" s="129"/>
+      <c r="P21" s="129"/>
+      <c r="Q21" s="129"/>
+      <c r="R21" s="129"/>
+      <c r="T21" s="129"/>
+      <c r="U21" s="129"/>
+      <c r="V21" s="129"/>
+      <c r="W21" s="129"/>
+      <c r="X21" s="129"/>
+      <c r="Y21" s="129"/>
+      <c r="Z21" s="129"/>
+      <c r="AA21" s="129"/>
+    </row>
+    <row r="22" spans="2:27" x14ac:dyDescent="0.2">
+      <c r="B22" s="129"/>
+      <c r="C22" s="129"/>
+      <c r="D22" s="129"/>
+      <c r="E22" s="129"/>
+      <c r="F22" s="129"/>
+      <c r="G22" s="129"/>
+      <c r="H22" s="129"/>
+      <c r="I22" s="129"/>
+      <c r="K22" s="129"/>
+      <c r="L22" s="129"/>
+      <c r="M22" s="129"/>
+      <c r="N22" s="129"/>
+      <c r="O22" s="129"/>
+      <c r="P22" s="129"/>
+      <c r="Q22" s="129"/>
+      <c r="R22" s="129"/>
+      <c r="T22" s="129"/>
+      <c r="U22" s="129"/>
+      <c r="V22" s="129"/>
+      <c r="W22" s="129"/>
+      <c r="X22" s="129"/>
+      <c r="Y22" s="129"/>
+      <c r="Z22" s="129"/>
+      <c r="AA22" s="129"/>
+    </row>
+    <row r="23" spans="2:27" x14ac:dyDescent="0.2">
+      <c r="B23" s="129"/>
+      <c r="C23" s="129"/>
+      <c r="D23" s="129"/>
+      <c r="E23" s="129"/>
+      <c r="F23" s="129"/>
+      <c r="G23" s="129"/>
+      <c r="H23" s="129"/>
+      <c r="I23" s="129"/>
+      <c r="K23" s="129"/>
+      <c r="L23" s="129"/>
+      <c r="M23" s="129"/>
+      <c r="N23" s="129"/>
+      <c r="O23" s="129"/>
+      <c r="P23" s="129"/>
+      <c r="Q23" s="129"/>
+      <c r="R23" s="129"/>
+      <c r="T23" s="129"/>
+      <c r="U23" s="129"/>
+      <c r="V23" s="129"/>
+      <c r="W23" s="129"/>
+      <c r="X23" s="129"/>
+      <c r="Y23" s="129"/>
+      <c r="Z23" s="129"/>
+      <c r="AA23" s="129"/>
+    </row>
+    <row r="24" spans="2:27" x14ac:dyDescent="0.2">
+      <c r="B24" s="129"/>
+      <c r="C24" s="129"/>
+      <c r="D24" s="129"/>
+      <c r="E24" s="129"/>
+      <c r="F24" s="129"/>
+      <c r="G24" s="129"/>
+      <c r="H24" s="129"/>
+      <c r="I24" s="129"/>
+      <c r="K24" s="129"/>
+      <c r="L24" s="129"/>
+      <c r="M24" s="129"/>
+      <c r="N24" s="129"/>
+      <c r="O24" s="129"/>
+      <c r="P24" s="129"/>
+      <c r="Q24" s="129"/>
+      <c r="R24" s="129"/>
+      <c r="T24" s="129"/>
+      <c r="U24" s="129"/>
+      <c r="V24" s="129"/>
+      <c r="W24" s="129"/>
+      <c r="X24" s="129"/>
+      <c r="Y24" s="129"/>
+      <c r="Z24" s="129"/>
+      <c r="AA24" s="129"/>
+    </row>
+    <row r="25" spans="2:27" x14ac:dyDescent="0.2">
+      <c r="B25" s="129"/>
+      <c r="C25" s="129"/>
+      <c r="D25" s="129"/>
+      <c r="E25" s="129"/>
+      <c r="F25" s="129"/>
+      <c r="G25" s="129"/>
+      <c r="H25" s="129"/>
+      <c r="I25" s="129"/>
+      <c r="K25" s="129"/>
+      <c r="L25" s="129"/>
+      <c r="M25" s="129"/>
+      <c r="N25" s="129"/>
+      <c r="O25" s="129"/>
+      <c r="P25" s="129"/>
+      <c r="Q25" s="129"/>
+      <c r="R25" s="129"/>
+      <c r="T25" s="129"/>
+      <c r="U25" s="129"/>
+      <c r="V25" s="129"/>
+      <c r="W25" s="129"/>
+      <c r="X25" s="129"/>
+      <c r="Y25" s="129"/>
+      <c r="Z25" s="129"/>
+      <c r="AA25" s="129"/>
+    </row>
+    <row r="26" spans="2:27" x14ac:dyDescent="0.2">
+      <c r="B26" s="129"/>
+      <c r="C26" s="129"/>
+      <c r="D26" s="129"/>
+      <c r="E26" s="129"/>
+      <c r="F26" s="129"/>
+      <c r="G26" s="129"/>
+      <c r="H26" s="129"/>
+      <c r="I26" s="129"/>
+      <c r="K26" s="129"/>
+      <c r="L26" s="129"/>
+      <c r="M26" s="129"/>
+      <c r="N26" s="129"/>
+      <c r="O26" s="129"/>
+      <c r="P26" s="129"/>
+      <c r="Q26" s="129"/>
+      <c r="R26" s="129"/>
+      <c r="T26" s="129"/>
+      <c r="U26" s="129"/>
+      <c r="V26" s="129"/>
+      <c r="W26" s="129"/>
+      <c r="X26" s="129"/>
+      <c r="Y26" s="129"/>
+      <c r="Z26" s="129"/>
+      <c r="AA26" s="129"/>
+    </row>
+    <row r="27" spans="2:27" x14ac:dyDescent="0.2">
+      <c r="B27" s="129"/>
+      <c r="C27" s="129"/>
+      <c r="D27" s="129"/>
+      <c r="E27" s="129"/>
+      <c r="F27" s="129"/>
+      <c r="G27" s="129"/>
+      <c r="H27" s="129"/>
+      <c r="I27" s="129"/>
+      <c r="K27" s="129"/>
+      <c r="L27" s="129"/>
+      <c r="M27" s="129"/>
+      <c r="N27" s="129"/>
+      <c r="O27" s="129"/>
+      <c r="P27" s="129"/>
+      <c r="Q27" s="129"/>
+      <c r="R27" s="129"/>
+      <c r="T27" s="129"/>
+      <c r="U27" s="129"/>
+      <c r="V27" s="129"/>
+      <c r="W27" s="129"/>
+      <c r="X27" s="129"/>
+      <c r="Y27" s="129"/>
+      <c r="Z27" s="129"/>
+      <c r="AA27" s="129"/>
+    </row>
+    <row r="28" spans="2:27" x14ac:dyDescent="0.2">
+      <c r="B28" s="129"/>
+      <c r="C28" s="129"/>
+      <c r="D28" s="129"/>
+      <c r="E28" s="129"/>
+      <c r="F28" s="129"/>
+      <c r="G28" s="129"/>
+      <c r="H28" s="129"/>
+      <c r="I28" s="129"/>
+      <c r="K28" s="129"/>
+      <c r="L28" s="129"/>
+      <c r="M28" s="129"/>
+      <c r="N28" s="129"/>
+      <c r="O28" s="129"/>
+      <c r="P28" s="129"/>
+      <c r="Q28" s="129"/>
+      <c r="R28" s="129"/>
+      <c r="T28" s="129"/>
+      <c r="U28" s="129"/>
+      <c r="V28" s="129"/>
+      <c r="W28" s="129"/>
+      <c r="X28" s="129"/>
+      <c r="Y28" s="129"/>
+      <c r="Z28" s="129"/>
+      <c r="AA28" s="129"/>
+    </row>
+    <row r="29" spans="2:27" x14ac:dyDescent="0.2">
+      <c r="B29" s="129"/>
+      <c r="C29" s="129"/>
+      <c r="D29" s="129"/>
+      <c r="E29" s="129"/>
+      <c r="F29" s="129"/>
+      <c r="G29" s="129"/>
+      <c r="H29" s="129"/>
+      <c r="I29" s="129"/>
+      <c r="K29" s="129"/>
+      <c r="L29" s="129"/>
+      <c r="M29" s="129"/>
+      <c r="N29" s="129"/>
+      <c r="O29" s="129"/>
+      <c r="P29" s="129"/>
+      <c r="Q29" s="129"/>
+      <c r="R29" s="129"/>
+      <c r="T29" s="129"/>
+      <c r="U29" s="129"/>
+      <c r="V29" s="129"/>
+      <c r="W29" s="129"/>
+      <c r="X29" s="129"/>
+      <c r="Y29" s="129"/>
+      <c r="Z29" s="129"/>
+      <c r="AA29" s="129"/>
+    </row>
+    <row r="30" spans="2:27" x14ac:dyDescent="0.2">
+      <c r="B30" s="129"/>
+      <c r="C30" s="129"/>
+      <c r="D30" s="129"/>
+      <c r="E30" s="129"/>
+      <c r="F30" s="129"/>
+      <c r="G30" s="129"/>
+      <c r="H30" s="129"/>
+      <c r="I30" s="129"/>
+      <c r="K30" s="129"/>
+      <c r="L30" s="129"/>
+      <c r="M30" s="129"/>
+      <c r="N30" s="129"/>
+      <c r="O30" s="129"/>
+      <c r="P30" s="129"/>
+      <c r="Q30" s="129"/>
+      <c r="R30" s="129"/>
+      <c r="T30" s="129"/>
+      <c r="U30" s="129"/>
+      <c r="V30" s="129"/>
+      <c r="W30" s="129"/>
+      <c r="X30" s="129"/>
+      <c r="Y30" s="129"/>
+      <c r="Z30" s="129"/>
+      <c r="AA30" s="129"/>
+    </row>
+    <row r="31" spans="2:27" x14ac:dyDescent="0.2">
+      <c r="B31" s="129"/>
+      <c r="C31" s="129"/>
+      <c r="D31" s="129"/>
+      <c r="E31" s="129"/>
+      <c r="F31" s="129"/>
+      <c r="G31" s="129"/>
+      <c r="H31" s="129"/>
+      <c r="I31" s="129"/>
+      <c r="K31" s="129"/>
+      <c r="L31" s="129"/>
+      <c r="M31" s="129"/>
+      <c r="N31" s="129"/>
+      <c r="O31" s="129"/>
+      <c r="P31" s="129"/>
+      <c r="Q31" s="129"/>
+      <c r="R31" s="129"/>
+      <c r="T31" s="129"/>
+      <c r="U31" s="129"/>
+      <c r="V31" s="129"/>
+      <c r="W31" s="129"/>
+      <c r="X31" s="129"/>
+      <c r="Y31" s="129"/>
+      <c r="Z31" s="129"/>
+      <c r="AA31" s="129"/>
+    </row>
+    <row r="32" spans="2:27" x14ac:dyDescent="0.2">
+      <c r="B32" s="129"/>
+      <c r="C32" s="129"/>
+      <c r="D32" s="129"/>
+      <c r="E32" s="129"/>
+      <c r="F32" s="129"/>
+      <c r="G32" s="129"/>
+      <c r="H32" s="129"/>
+      <c r="I32" s="129"/>
+      <c r="K32" s="129"/>
+      <c r="L32" s="129"/>
+      <c r="M32" s="129"/>
+      <c r="N32" s="129"/>
+      <c r="O32" s="129"/>
+      <c r="P32" s="129"/>
+      <c r="Q32" s="129"/>
+      <c r="R32" s="129"/>
+      <c r="T32" s="129"/>
+      <c r="U32" s="129"/>
+      <c r="V32" s="129"/>
+      <c r="W32" s="129"/>
+      <c r="X32" s="129"/>
+      <c r="Y32" s="129"/>
+      <c r="Z32" s="129"/>
+      <c r="AA32" s="129"/>
+    </row>
+    <row r="33" spans="2:27" x14ac:dyDescent="0.2">
+      <c r="B33" s="129"/>
+      <c r="C33" s="129"/>
+      <c r="D33" s="129"/>
+      <c r="E33" s="129"/>
+      <c r="F33" s="129"/>
+      <c r="G33" s="129"/>
+      <c r="H33" s="129"/>
+      <c r="I33" s="129"/>
+      <c r="K33" s="129"/>
+      <c r="L33" s="129"/>
+      <c r="M33" s="129"/>
+      <c r="N33" s="129"/>
+      <c r="O33" s="129"/>
+      <c r="P33" s="129"/>
+      <c r="Q33" s="129"/>
+      <c r="R33" s="129"/>
+      <c r="T33" s="129"/>
+      <c r="U33" s="129"/>
+      <c r="V33" s="129"/>
+      <c r="W33" s="129"/>
+      <c r="X33" s="129"/>
+      <c r="Y33" s="129"/>
+      <c r="Z33" s="129"/>
+      <c r="AA33" s="129"/>
+    </row>
+    <row r="34" spans="2:27" x14ac:dyDescent="0.2">
+      <c r="B34" s="129"/>
+      <c r="C34" s="129"/>
+      <c r="D34" s="129"/>
+      <c r="E34" s="129"/>
+      <c r="F34" s="129"/>
+      <c r="G34" s="129"/>
+      <c r="H34" s="129"/>
+      <c r="I34" s="129"/>
+      <c r="K34" s="129"/>
+      <c r="L34" s="129"/>
+      <c r="M34" s="129"/>
+      <c r="N34" s="129"/>
+      <c r="O34" s="129"/>
+      <c r="P34" s="129"/>
+      <c r="Q34" s="129"/>
+      <c r="R34" s="129"/>
+      <c r="T34" s="129"/>
+      <c r="U34" s="129"/>
+      <c r="V34" s="129"/>
+      <c r="W34" s="129"/>
+      <c r="X34" s="129"/>
+      <c r="Y34" s="129"/>
+      <c r="Z34" s="129"/>
+      <c r="AA34" s="129"/>
+    </row>
+    <row r="35" spans="2:27" x14ac:dyDescent="0.2">
+      <c r="B35" s="129"/>
+      <c r="C35" s="129"/>
+      <c r="D35" s="129"/>
+      <c r="E35" s="129"/>
+      <c r="F35" s="129"/>
+      <c r="G35" s="129"/>
+      <c r="H35" s="129"/>
+      <c r="I35" s="129"/>
+      <c r="K35" s="129"/>
+      <c r="L35" s="129"/>
+      <c r="M35" s="129"/>
+      <c r="N35" s="129"/>
+      <c r="O35" s="129"/>
+      <c r="P35" s="129"/>
+      <c r="Q35" s="129"/>
+      <c r="R35" s="129"/>
+      <c r="T35" s="129"/>
+      <c r="U35" s="129"/>
+      <c r="V35" s="129"/>
+      <c r="W35" s="129"/>
+      <c r="X35" s="129"/>
+      <c r="Y35" s="129"/>
+      <c r="Z35" s="129"/>
+      <c r="AA35" s="129"/>
+    </row>
+    <row r="36" spans="2:27" x14ac:dyDescent="0.2">
+      <c r="B36" s="129"/>
+      <c r="C36" s="129"/>
+      <c r="D36" s="129"/>
+      <c r="E36" s="129"/>
+      <c r="F36" s="129"/>
+      <c r="G36" s="129"/>
+      <c r="H36" s="129"/>
+      <c r="I36" s="129"/>
+      <c r="K36" s="129"/>
+      <c r="L36" s="129"/>
+      <c r="M36" s="129"/>
+      <c r="N36" s="129"/>
+      <c r="O36" s="129"/>
+      <c r="P36" s="129"/>
+      <c r="Q36" s="129"/>
+      <c r="R36" s="129"/>
+      <c r="T36" s="129"/>
+      <c r="U36" s="129"/>
+      <c r="V36" s="129"/>
+      <c r="W36" s="129"/>
+      <c r="X36" s="129"/>
+      <c r="Y36" s="129"/>
+      <c r="Z36" s="129"/>
+      <c r="AA36" s="129"/>
+    </row>
+    <row r="37" spans="2:27" x14ac:dyDescent="0.2">
+      <c r="B37" s="129"/>
+      <c r="C37" s="129"/>
+      <c r="D37" s="129"/>
+      <c r="E37" s="129"/>
+      <c r="F37" s="129"/>
+      <c r="G37" s="129"/>
+      <c r="H37" s="129"/>
+      <c r="I37" s="129"/>
+      <c r="K37" s="129"/>
+      <c r="L37" s="129"/>
+      <c r="M37" s="129"/>
+      <c r="N37" s="129"/>
+      <c r="O37" s="129"/>
+      <c r="P37" s="129"/>
+      <c r="Q37" s="129"/>
+      <c r="R37" s="129"/>
+      <c r="T37" s="129"/>
+      <c r="U37" s="129"/>
+      <c r="V37" s="129"/>
+      <c r="W37" s="129"/>
+      <c r="X37" s="129"/>
+      <c r="Y37" s="129"/>
+      <c r="Z37" s="129"/>
+      <c r="AA37" s="129"/>
+    </row>
+    <row r="38" spans="2:27" x14ac:dyDescent="0.2">
+      <c r="B38" s="129"/>
+      <c r="C38" s="129"/>
+      <c r="D38" s="129"/>
+      <c r="E38" s="129"/>
+      <c r="F38" s="129"/>
+      <c r="G38" s="129"/>
+      <c r="H38" s="129"/>
+      <c r="I38" s="129"/>
+      <c r="K38" s="129"/>
+      <c r="L38" s="129"/>
+      <c r="M38" s="129"/>
+      <c r="N38" s="129"/>
+      <c r="O38" s="129"/>
+      <c r="P38" s="129"/>
+      <c r="Q38" s="129"/>
+      <c r="R38" s="129"/>
+      <c r="T38" s="129"/>
+      <c r="U38" s="129"/>
+      <c r="V38" s="129"/>
+      <c r="W38" s="129"/>
+      <c r="X38" s="129"/>
+      <c r="Y38" s="129"/>
+      <c r="Z38" s="129"/>
+      <c r="AA38" s="129"/>
+    </row>
+    <row r="39" spans="2:27" x14ac:dyDescent="0.2">
+      <c r="B39" s="129"/>
+      <c r="C39" s="129"/>
+      <c r="D39" s="129"/>
+      <c r="E39" s="129"/>
+      <c r="F39" s="129"/>
+      <c r="G39" s="129"/>
+      <c r="H39" s="129"/>
+      <c r="I39" s="129"/>
+      <c r="K39" s="129"/>
+      <c r="L39" s="129"/>
+      <c r="M39" s="129"/>
+      <c r="N39" s="129"/>
+      <c r="O39" s="129"/>
+      <c r="P39" s="129"/>
+      <c r="Q39" s="129"/>
+      <c r="R39" s="129"/>
+      <c r="T39" s="129"/>
+      <c r="U39" s="129"/>
+      <c r="V39" s="129"/>
+      <c r="W39" s="129"/>
+      <c r="X39" s="129"/>
+      <c r="Y39" s="129"/>
+      <c r="Z39" s="129"/>
+      <c r="AA39" s="129"/>
+    </row>
+    <row r="40" spans="2:27" x14ac:dyDescent="0.2">
+      <c r="B40" s="129"/>
+      <c r="C40" s="129"/>
+      <c r="D40" s="129"/>
+      <c r="E40" s="129"/>
+      <c r="F40" s="129"/>
+      <c r="G40" s="129"/>
+      <c r="H40" s="129"/>
+      <c r="I40" s="129"/>
+      <c r="K40" s="129"/>
+      <c r="L40" s="129"/>
+      <c r="M40" s="129"/>
+      <c r="N40" s="129"/>
+      <c r="O40" s="129"/>
+      <c r="P40" s="129"/>
+      <c r="Q40" s="129"/>
+      <c r="R40" s="129"/>
+      <c r="T40" s="129"/>
+      <c r="U40" s="129"/>
+      <c r="V40" s="129"/>
+      <c r="W40" s="129"/>
+      <c r="X40" s="129"/>
+      <c r="Y40" s="129"/>
+      <c r="Z40" s="129"/>
+      <c r="AA40" s="129"/>
+    </row>
+    <row r="41" spans="2:27" x14ac:dyDescent="0.2">
+      <c r="B41" s="129"/>
+      <c r="C41" s="129"/>
+      <c r="D41" s="129"/>
+      <c r="E41" s="129"/>
+      <c r="F41" s="129"/>
+      <c r="G41" s="129"/>
+      <c r="H41" s="129"/>
+      <c r="I41" s="129"/>
+      <c r="K41" s="129"/>
+      <c r="L41" s="129"/>
+      <c r="M41" s="129"/>
+      <c r="N41" s="129"/>
+      <c r="O41" s="129"/>
+      <c r="P41" s="129"/>
+      <c r="Q41" s="129"/>
+      <c r="R41" s="129"/>
+      <c r="T41" s="129"/>
+      <c r="U41" s="129"/>
+      <c r="V41" s="129"/>
+      <c r="W41" s="129"/>
+      <c r="X41" s="129"/>
+      <c r="Y41" s="129"/>
+      <c r="Z41" s="129"/>
+      <c r="AA41" s="129"/>
+    </row>
+    <row r="42" spans="2:27" x14ac:dyDescent="0.2">
+      <c r="B42" s="129"/>
+      <c r="C42" s="129"/>
+      <c r="D42" s="129"/>
+      <c r="E42" s="129"/>
+      <c r="F42" s="129"/>
+      <c r="G42" s="129"/>
+      <c r="H42" s="129"/>
+      <c r="I42" s="129"/>
+      <c r="K42" s="129"/>
+      <c r="L42" s="129"/>
+      <c r="M42" s="129"/>
+      <c r="N42" s="129"/>
+      <c r="O42" s="129"/>
+      <c r="P42" s="129"/>
+      <c r="Q42" s="129"/>
+      <c r="R42" s="129"/>
+      <c r="T42" s="129"/>
+      <c r="U42" s="129"/>
+      <c r="V42" s="129"/>
+      <c r="W42" s="129"/>
+      <c r="X42" s="129"/>
+      <c r="Y42" s="129"/>
+      <c r="Z42" s="129"/>
+      <c r="AA42" s="129"/>
+    </row>
+  </sheetData>
+  <mergeCells count="15">
+    <mergeCell ref="K16:R16"/>
+    <mergeCell ref="K17:K19"/>
+    <mergeCell ref="L17:M17"/>
+    <mergeCell ref="N17:R17"/>
+    <mergeCell ref="L19:M19"/>
+    <mergeCell ref="T16:AA16"/>
+    <mergeCell ref="T17:T19"/>
+    <mergeCell ref="U17:V17"/>
+    <mergeCell ref="W17:AA17"/>
+    <mergeCell ref="U19:V19"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="B17:B19"/>
+    <mergeCell ref="E17:I17"/>
+    <mergeCell ref="B16:I16"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Feuille5" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -18933,9 +19816,9 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Feuille3" enableFormatConditionsCalculation="0"/>
+  <sheetPr codeName="Feuille6" enableFormatConditionsCalculation="0"/>
   <dimension ref="C1:Z56"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -18956,14 +19839,14 @@
       <c r="F1" s="53"/>
       <c r="G1" s="53"/>
       <c r="H1" s="53"/>
-      <c r="I1" s="98" t="s">
+      <c r="I1" s="115" t="s">
         <v>80</v>
       </c>
-      <c r="J1" s="98"/>
-      <c r="K1" s="98"/>
-      <c r="L1" s="98"/>
-      <c r="M1" s="98"/>
-      <c r="N1" s="98"/>
+      <c r="J1" s="115"/>
+      <c r="K1" s="115"/>
+      <c r="L1" s="115"/>
+      <c r="M1" s="115"/>
+      <c r="N1" s="115"/>
       <c r="O1" s="54"/>
       <c r="P1" s="54"/>
       <c r="Q1" s="54"/>
@@ -18984,12 +19867,12 @@
       <c r="F2" s="53"/>
       <c r="G2" s="54"/>
       <c r="H2" s="53"/>
-      <c r="I2" s="98"/>
-      <c r="J2" s="98"/>
-      <c r="K2" s="98"/>
-      <c r="L2" s="98"/>
-      <c r="M2" s="98"/>
-      <c r="N2" s="98"/>
+      <c r="I2" s="115"/>
+      <c r="J2" s="115"/>
+      <c r="K2" s="115"/>
+      <c r="L2" s="115"/>
+      <c r="M2" s="115"/>
+      <c r="N2" s="115"/>
       <c r="O2" s="54"/>
       <c r="P2" s="54"/>
       <c r="Q2" s="54"/>
@@ -19016,16 +19899,16 @@
         <f>Import_GoogleForm!H3</f>
         <v>5</v>
       </c>
-      <c r="J3" s="99">
+      <c r="J3" s="116">
         <f>Import_GoogleForm!L3</f>
         <v>43129</v>
       </c>
-      <c r="K3" s="99"/>
-      <c r="L3" s="100">
+      <c r="K3" s="116"/>
+      <c r="L3" s="117">
         <f>J3+6</f>
         <v>43135</v>
       </c>
-      <c r="M3" s="100"/>
+      <c r="M3" s="117"/>
       <c r="N3" s="59"/>
       <c r="O3" s="54"/>
       <c r="P3" s="54"/>
@@ -19070,24 +19953,24 @@
     </row>
     <row r="5" spans="3:26" ht="16" x14ac:dyDescent="0.2">
       <c r="C5" s="52"/>
-      <c r="D5" s="101" t="s">
+      <c r="D5" s="118" t="s">
         <v>83</v>
       </c>
-      <c r="E5" s="102"/>
-      <c r="F5" s="102"/>
+      <c r="E5" s="119"/>
+      <c r="F5" s="119"/>
       <c r="G5" s="54"/>
-      <c r="H5" s="103" t="s">
+      <c r="H5" s="120" t="s">
         <v>84</v>
       </c>
-      <c r="I5" s="104"/>
-      <c r="J5" s="104"/>
+      <c r="I5" s="121"/>
+      <c r="J5" s="121"/>
       <c r="K5" s="54"/>
       <c r="L5" s="54"/>
-      <c r="M5" s="105" t="s">
+      <c r="M5" s="122" t="s">
         <v>85</v>
       </c>
-      <c r="N5" s="102"/>
-      <c r="O5" s="102"/>
+      <c r="N5" s="119"/>
+      <c r="O5" s="119"/>
       <c r="P5" s="54"/>
       <c r="Q5" s="54"/>
       <c r="R5" s="63" t="s">
@@ -19130,31 +20013,31 @@
     </row>
     <row r="7" spans="3:26" x14ac:dyDescent="0.2">
       <c r="C7" s="52"/>
-      <c r="D7" s="95">
+      <c r="D7" s="112">
         <f>Import_GoogleForm!L3</f>
         <v>43129</v>
       </c>
-      <c r="E7" s="96"/>
-      <c r="F7" s="96"/>
-      <c r="G7" s="96"/>
-      <c r="H7" s="96"/>
-      <c r="I7" s="96"/>
-      <c r="J7" s="96"/>
-      <c r="K7" s="96"/>
-      <c r="L7" s="96"/>
-      <c r="M7" s="96"/>
-      <c r="N7" s="96"/>
-      <c r="O7" s="96"/>
-      <c r="P7" s="96"/>
-      <c r="Q7" s="96"/>
-      <c r="R7" s="96"/>
-      <c r="S7" s="96"/>
-      <c r="T7" s="96"/>
-      <c r="U7" s="96"/>
-      <c r="V7" s="96"/>
-      <c r="W7" s="96"/>
-      <c r="X7" s="96"/>
-      <c r="Y7" s="97"/>
+      <c r="E7" s="113"/>
+      <c r="F7" s="113"/>
+      <c r="G7" s="113"/>
+      <c r="H7" s="113"/>
+      <c r="I7" s="113"/>
+      <c r="J7" s="113"/>
+      <c r="K7" s="113"/>
+      <c r="L7" s="113"/>
+      <c r="M7" s="113"/>
+      <c r="N7" s="113"/>
+      <c r="O7" s="113"/>
+      <c r="P7" s="113"/>
+      <c r="Q7" s="113"/>
+      <c r="R7" s="113"/>
+      <c r="S7" s="113"/>
+      <c r="T7" s="113"/>
+      <c r="U7" s="113"/>
+      <c r="V7" s="113"/>
+      <c r="W7" s="113"/>
+      <c r="X7" s="113"/>
+      <c r="Y7" s="114"/>
       <c r="Z7" s="53"/>
     </row>
     <row r="8" spans="3:26" x14ac:dyDescent="0.2">
@@ -19543,31 +20426,31 @@
     </row>
     <row r="14" spans="3:26" x14ac:dyDescent="0.2">
       <c r="C14" s="52"/>
-      <c r="D14" s="95">
+      <c r="D14" s="112">
         <f>D7+1</f>
         <v>43130</v>
       </c>
-      <c r="E14" s="96"/>
-      <c r="F14" s="96"/>
-      <c r="G14" s="96"/>
-      <c r="H14" s="96"/>
-      <c r="I14" s="96"/>
-      <c r="J14" s="96"/>
-      <c r="K14" s="96"/>
-      <c r="L14" s="96"/>
-      <c r="M14" s="96"/>
-      <c r="N14" s="96"/>
-      <c r="O14" s="96"/>
-      <c r="P14" s="96"/>
-      <c r="Q14" s="96"/>
-      <c r="R14" s="96"/>
-      <c r="S14" s="96"/>
-      <c r="T14" s="96"/>
-      <c r="U14" s="96"/>
-      <c r="V14" s="96"/>
-      <c r="W14" s="96"/>
-      <c r="X14" s="96"/>
-      <c r="Y14" s="97"/>
+      <c r="E14" s="113"/>
+      <c r="F14" s="113"/>
+      <c r="G14" s="113"/>
+      <c r="H14" s="113"/>
+      <c r="I14" s="113"/>
+      <c r="J14" s="113"/>
+      <c r="K14" s="113"/>
+      <c r="L14" s="113"/>
+      <c r="M14" s="113"/>
+      <c r="N14" s="113"/>
+      <c r="O14" s="113"/>
+      <c r="P14" s="113"/>
+      <c r="Q14" s="113"/>
+      <c r="R14" s="113"/>
+      <c r="S14" s="113"/>
+      <c r="T14" s="113"/>
+      <c r="U14" s="113"/>
+      <c r="V14" s="113"/>
+      <c r="W14" s="113"/>
+      <c r="X14" s="113"/>
+      <c r="Y14" s="114"/>
       <c r="Z14" s="53"/>
     </row>
     <row r="15" spans="3:26" x14ac:dyDescent="0.2">
@@ -19955,31 +20838,31 @@
     </row>
     <row r="21" spans="3:26" x14ac:dyDescent="0.2">
       <c r="C21" s="52"/>
-      <c r="D21" s="95">
+      <c r="D21" s="112">
         <f>D14+1</f>
         <v>43131</v>
       </c>
-      <c r="E21" s="96"/>
-      <c r="F21" s="96"/>
-      <c r="G21" s="96"/>
-      <c r="H21" s="96"/>
-      <c r="I21" s="96"/>
-      <c r="J21" s="96"/>
-      <c r="K21" s="96"/>
-      <c r="L21" s="96"/>
-      <c r="M21" s="96"/>
-      <c r="N21" s="96"/>
-      <c r="O21" s="96"/>
-      <c r="P21" s="96"/>
-      <c r="Q21" s="96"/>
-      <c r="R21" s="96"/>
-      <c r="S21" s="96"/>
-      <c r="T21" s="96"/>
-      <c r="U21" s="96"/>
-      <c r="V21" s="96"/>
-      <c r="W21" s="96"/>
-      <c r="X21" s="96"/>
-      <c r="Y21" s="97"/>
+      <c r="E21" s="113"/>
+      <c r="F21" s="113"/>
+      <c r="G21" s="113"/>
+      <c r="H21" s="113"/>
+      <c r="I21" s="113"/>
+      <c r="J21" s="113"/>
+      <c r="K21" s="113"/>
+      <c r="L21" s="113"/>
+      <c r="M21" s="113"/>
+      <c r="N21" s="113"/>
+      <c r="O21" s="113"/>
+      <c r="P21" s="113"/>
+      <c r="Q21" s="113"/>
+      <c r="R21" s="113"/>
+      <c r="S21" s="113"/>
+      <c r="T21" s="113"/>
+      <c r="U21" s="113"/>
+      <c r="V21" s="113"/>
+      <c r="W21" s="113"/>
+      <c r="X21" s="113"/>
+      <c r="Y21" s="114"/>
       <c r="Z21" s="53"/>
     </row>
     <row r="22" spans="3:26" x14ac:dyDescent="0.2">
@@ -20367,31 +21250,31 @@
     </row>
     <row r="28" spans="3:26" x14ac:dyDescent="0.2">
       <c r="C28" s="52"/>
-      <c r="D28" s="95">
+      <c r="D28" s="112">
         <f>D21+1</f>
         <v>43132</v>
       </c>
-      <c r="E28" s="96"/>
-      <c r="F28" s="96"/>
-      <c r="G28" s="96"/>
-      <c r="H28" s="96"/>
-      <c r="I28" s="96"/>
-      <c r="J28" s="96"/>
-      <c r="K28" s="96"/>
-      <c r="L28" s="96"/>
-      <c r="M28" s="96"/>
-      <c r="N28" s="96"/>
-      <c r="O28" s="96"/>
-      <c r="P28" s="96"/>
-      <c r="Q28" s="96"/>
-      <c r="R28" s="96"/>
-      <c r="S28" s="96"/>
-      <c r="T28" s="96"/>
-      <c r="U28" s="96"/>
-      <c r="V28" s="96"/>
-      <c r="W28" s="96"/>
-      <c r="X28" s="96"/>
-      <c r="Y28" s="97"/>
+      <c r="E28" s="113"/>
+      <c r="F28" s="113"/>
+      <c r="G28" s="113"/>
+      <c r="H28" s="113"/>
+      <c r="I28" s="113"/>
+      <c r="J28" s="113"/>
+      <c r="K28" s="113"/>
+      <c r="L28" s="113"/>
+      <c r="M28" s="113"/>
+      <c r="N28" s="113"/>
+      <c r="O28" s="113"/>
+      <c r="P28" s="113"/>
+      <c r="Q28" s="113"/>
+      <c r="R28" s="113"/>
+      <c r="S28" s="113"/>
+      <c r="T28" s="113"/>
+      <c r="U28" s="113"/>
+      <c r="V28" s="113"/>
+      <c r="W28" s="113"/>
+      <c r="X28" s="113"/>
+      <c r="Y28" s="114"/>
       <c r="Z28" s="53"/>
     </row>
     <row r="29" spans="3:26" x14ac:dyDescent="0.2">
@@ -20779,31 +21662,31 @@
     </row>
     <row r="35" spans="3:26" x14ac:dyDescent="0.2">
       <c r="C35" s="52"/>
-      <c r="D35" s="95">
+      <c r="D35" s="112">
         <f>D28+1</f>
         <v>43133</v>
       </c>
-      <c r="E35" s="96"/>
-      <c r="F35" s="96"/>
-      <c r="G35" s="96"/>
-      <c r="H35" s="96"/>
-      <c r="I35" s="96"/>
-      <c r="J35" s="96"/>
-      <c r="K35" s="96"/>
-      <c r="L35" s="96"/>
-      <c r="M35" s="96"/>
-      <c r="N35" s="96"/>
-      <c r="O35" s="96"/>
-      <c r="P35" s="96"/>
-      <c r="Q35" s="96"/>
-      <c r="R35" s="96"/>
-      <c r="S35" s="96"/>
-      <c r="T35" s="96"/>
-      <c r="U35" s="96"/>
-      <c r="V35" s="96"/>
-      <c r="W35" s="96"/>
-      <c r="X35" s="96"/>
-      <c r="Y35" s="97"/>
+      <c r="E35" s="113"/>
+      <c r="F35" s="113"/>
+      <c r="G35" s="113"/>
+      <c r="H35" s="113"/>
+      <c r="I35" s="113"/>
+      <c r="J35" s="113"/>
+      <c r="K35" s="113"/>
+      <c r="L35" s="113"/>
+      <c r="M35" s="113"/>
+      <c r="N35" s="113"/>
+      <c r="O35" s="113"/>
+      <c r="P35" s="113"/>
+      <c r="Q35" s="113"/>
+      <c r="R35" s="113"/>
+      <c r="S35" s="113"/>
+      <c r="T35" s="113"/>
+      <c r="U35" s="113"/>
+      <c r="V35" s="113"/>
+      <c r="W35" s="113"/>
+      <c r="X35" s="113"/>
+      <c r="Y35" s="114"/>
       <c r="Z35" s="53"/>
     </row>
     <row r="36" spans="3:26" x14ac:dyDescent="0.2">
@@ -21191,31 +22074,31 @@
     </row>
     <row r="42" spans="3:26" x14ac:dyDescent="0.2">
       <c r="C42" s="52"/>
-      <c r="D42" s="95">
+      <c r="D42" s="112">
         <f>D35+1</f>
         <v>43134</v>
       </c>
-      <c r="E42" s="96"/>
-      <c r="F42" s="96"/>
-      <c r="G42" s="96"/>
-      <c r="H42" s="96"/>
-      <c r="I42" s="96"/>
-      <c r="J42" s="96"/>
-      <c r="K42" s="96"/>
-      <c r="L42" s="96"/>
-      <c r="M42" s="96"/>
-      <c r="N42" s="96"/>
-      <c r="O42" s="96"/>
-      <c r="P42" s="96"/>
-      <c r="Q42" s="96"/>
-      <c r="R42" s="96"/>
-      <c r="S42" s="96"/>
-      <c r="T42" s="96"/>
-      <c r="U42" s="96"/>
-      <c r="V42" s="96"/>
-      <c r="W42" s="96"/>
-      <c r="X42" s="96"/>
-      <c r="Y42" s="97"/>
+      <c r="E42" s="113"/>
+      <c r="F42" s="113"/>
+      <c r="G42" s="113"/>
+      <c r="H42" s="113"/>
+      <c r="I42" s="113"/>
+      <c r="J42" s="113"/>
+      <c r="K42" s="113"/>
+      <c r="L42" s="113"/>
+      <c r="M42" s="113"/>
+      <c r="N42" s="113"/>
+      <c r="O42" s="113"/>
+      <c r="P42" s="113"/>
+      <c r="Q42" s="113"/>
+      <c r="R42" s="113"/>
+      <c r="S42" s="113"/>
+      <c r="T42" s="113"/>
+      <c r="U42" s="113"/>
+      <c r="V42" s="113"/>
+      <c r="W42" s="113"/>
+      <c r="X42" s="113"/>
+      <c r="Y42" s="114"/>
       <c r="Z42" s="53"/>
     </row>
     <row r="43" spans="3:26" x14ac:dyDescent="0.2">
@@ -21603,31 +22486,31 @@
     </row>
     <row r="49" spans="3:26" x14ac:dyDescent="0.2">
       <c r="C49" s="52"/>
-      <c r="D49" s="95">
+      <c r="D49" s="112">
         <f>D42+1</f>
         <v>43135</v>
       </c>
-      <c r="E49" s="96"/>
-      <c r="F49" s="96"/>
-      <c r="G49" s="96"/>
-      <c r="H49" s="96"/>
-      <c r="I49" s="96"/>
-      <c r="J49" s="96"/>
-      <c r="K49" s="96"/>
-      <c r="L49" s="96"/>
-      <c r="M49" s="96"/>
-      <c r="N49" s="96"/>
-      <c r="O49" s="96"/>
-      <c r="P49" s="96"/>
-      <c r="Q49" s="96"/>
-      <c r="R49" s="96"/>
-      <c r="S49" s="96"/>
-      <c r="T49" s="96"/>
-      <c r="U49" s="96"/>
-      <c r="V49" s="96"/>
-      <c r="W49" s="96"/>
-      <c r="X49" s="96"/>
-      <c r="Y49" s="97"/>
+      <c r="E49" s="113"/>
+      <c r="F49" s="113"/>
+      <c r="G49" s="113"/>
+      <c r="H49" s="113"/>
+      <c r="I49" s="113"/>
+      <c r="J49" s="113"/>
+      <c r="K49" s="113"/>
+      <c r="L49" s="113"/>
+      <c r="M49" s="113"/>
+      <c r="N49" s="113"/>
+      <c r="O49" s="113"/>
+      <c r="P49" s="113"/>
+      <c r="Q49" s="113"/>
+      <c r="R49" s="113"/>
+      <c r="S49" s="113"/>
+      <c r="T49" s="113"/>
+      <c r="U49" s="113"/>
+      <c r="V49" s="113"/>
+      <c r="W49" s="113"/>
+      <c r="X49" s="113"/>
+      <c r="Y49" s="114"/>
       <c r="Z49" s="53"/>
     </row>
     <row r="50" spans="3:26" x14ac:dyDescent="0.2">
@@ -22446,12 +23329,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Feuille4" enableFormatConditionsCalculation="0"/>
+  <sheetPr codeName="Feuille7" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:FD63"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -22473,326 +23356,326 @@
       <c r="A2" s="17" t="s">
         <v>56</v>
       </c>
-      <c r="B2" s="109" t="s">
+      <c r="B2" s="126" t="s">
         <v>57</v>
       </c>
-      <c r="C2" s="110" t="s">
+      <c r="C2" s="127" t="s">
         <v>58</v>
       </c>
-      <c r="D2" s="111" t="s">
+      <c r="D2" s="128" t="s">
         <v>59</v>
       </c>
-      <c r="E2" s="106">
+      <c r="E2" s="123">
         <v>1</v>
       </c>
-      <c r="F2" s="107"/>
-      <c r="G2" s="108"/>
-      <c r="H2" s="106">
+      <c r="F2" s="124"/>
+      <c r="G2" s="125"/>
+      <c r="H2" s="123">
         <f>E2+1</f>
         <v>2</v>
       </c>
-      <c r="I2" s="107"/>
-      <c r="J2" s="108"/>
-      <c r="K2" s="106">
-        <f t="shared" ref="K2" si="0">H2+1</f>
+      <c r="I2" s="124"/>
+      <c r="J2" s="125"/>
+      <c r="K2" s="123">
+        <f>H2+1</f>
         <v>3</v>
       </c>
-      <c r="L2" s="107"/>
-      <c r="M2" s="108"/>
-      <c r="N2" s="106">
-        <f t="shared" ref="N2" si="1">K2+1</f>
+      <c r="L2" s="124"/>
+      <c r="M2" s="125"/>
+      <c r="N2" s="123">
+        <f>K2+1</f>
         <v>4</v>
       </c>
-      <c r="O2" s="107"/>
-      <c r="P2" s="108"/>
-      <c r="Q2" s="106">
-        <f t="shared" ref="Q2" si="2">N2+1</f>
+      <c r="O2" s="124"/>
+      <c r="P2" s="125"/>
+      <c r="Q2" s="123">
+        <f>N2+1</f>
         <v>5</v>
       </c>
-      <c r="R2" s="107"/>
-      <c r="S2" s="108"/>
-      <c r="T2" s="106">
-        <f t="shared" ref="T2" si="3">Q2+1</f>
+      <c r="R2" s="124"/>
+      <c r="S2" s="125"/>
+      <c r="T2" s="123">
+        <f>Q2+1</f>
         <v>6</v>
       </c>
-      <c r="U2" s="107"/>
-      <c r="V2" s="108"/>
-      <c r="W2" s="106">
-        <f t="shared" ref="W2" si="4">T2+1</f>
+      <c r="U2" s="124"/>
+      <c r="V2" s="125"/>
+      <c r="W2" s="123">
+        <f>T2+1</f>
         <v>7</v>
       </c>
-      <c r="X2" s="107"/>
-      <c r="Y2" s="108"/>
-      <c r="Z2" s="106">
-        <f t="shared" ref="Z2" si="5">W2+1</f>
+      <c r="X2" s="124"/>
+      <c r="Y2" s="125"/>
+      <c r="Z2" s="123">
+        <f>W2+1</f>
         <v>8</v>
       </c>
-      <c r="AA2" s="107"/>
-      <c r="AB2" s="108"/>
-      <c r="AC2" s="106">
-        <f t="shared" ref="AC2" si="6">Z2+1</f>
+      <c r="AA2" s="124"/>
+      <c r="AB2" s="125"/>
+      <c r="AC2" s="123">
+        <f>Z2+1</f>
         <v>9</v>
       </c>
-      <c r="AD2" s="107"/>
-      <c r="AE2" s="108"/>
-      <c r="AF2" s="106">
+      <c r="AD2" s="124"/>
+      <c r="AE2" s="125"/>
+      <c r="AF2" s="123">
         <f>AC2+1</f>
         <v>10</v>
       </c>
-      <c r="AG2" s="107"/>
-      <c r="AH2" s="108"/>
-      <c r="AI2" s="106">
-        <f t="shared" ref="AI2" si="7">AF2+1</f>
+      <c r="AG2" s="124"/>
+      <c r="AH2" s="125"/>
+      <c r="AI2" s="123">
+        <f>AF2+1</f>
         <v>11</v>
       </c>
-      <c r="AJ2" s="107"/>
-      <c r="AK2" s="108"/>
-      <c r="AL2" s="106">
-        <f t="shared" ref="AL2" si="8">AI2+1</f>
+      <c r="AJ2" s="124"/>
+      <c r="AK2" s="125"/>
+      <c r="AL2" s="123">
+        <f>AI2+1</f>
         <v>12</v>
       </c>
-      <c r="AM2" s="107"/>
-      <c r="AN2" s="108"/>
-      <c r="AO2" s="106">
-        <f t="shared" ref="AO2" si="9">AL2+1</f>
+      <c r="AM2" s="124"/>
+      <c r="AN2" s="125"/>
+      <c r="AO2" s="123">
+        <f>AL2+1</f>
         <v>13</v>
       </c>
-      <c r="AP2" s="107"/>
-      <c r="AQ2" s="108"/>
-      <c r="AR2" s="106">
-        <f t="shared" ref="AR2" si="10">AO2+1</f>
+      <c r="AP2" s="124"/>
+      <c r="AQ2" s="125"/>
+      <c r="AR2" s="123">
+        <f>AO2+1</f>
         <v>14</v>
       </c>
-      <c r="AS2" s="107"/>
-      <c r="AT2" s="108"/>
-      <c r="AU2" s="106">
-        <f t="shared" ref="AU2" si="11">AR2+1</f>
+      <c r="AS2" s="124"/>
+      <c r="AT2" s="125"/>
+      <c r="AU2" s="123">
+        <f>AR2+1</f>
         <v>15</v>
       </c>
-      <c r="AV2" s="107"/>
-      <c r="AW2" s="108"/>
-      <c r="AX2" s="106">
-        <f t="shared" ref="AX2" si="12">AU2+1</f>
+      <c r="AV2" s="124"/>
+      <c r="AW2" s="125"/>
+      <c r="AX2" s="123">
+        <f>AU2+1</f>
         <v>16</v>
       </c>
-      <c r="AY2" s="107"/>
-      <c r="AZ2" s="108"/>
-      <c r="BA2" s="106">
-        <f t="shared" ref="BA2" si="13">AX2+1</f>
+      <c r="AY2" s="124"/>
+      <c r="AZ2" s="125"/>
+      <c r="BA2" s="123">
+        <f>AX2+1</f>
         <v>17</v>
       </c>
-      <c r="BB2" s="107"/>
-      <c r="BC2" s="108"/>
-      <c r="BD2" s="106">
+      <c r="BB2" s="124"/>
+      <c r="BC2" s="125"/>
+      <c r="BD2" s="123">
         <f>BA2+1</f>
         <v>18</v>
       </c>
-      <c r="BE2" s="107"/>
-      <c r="BF2" s="108"/>
-      <c r="BG2" s="106">
-        <f t="shared" ref="BG2" si="14">BD2+1</f>
+      <c r="BE2" s="124"/>
+      <c r="BF2" s="125"/>
+      <c r="BG2" s="123">
+        <f>BD2+1</f>
         <v>19</v>
       </c>
-      <c r="BH2" s="107"/>
-      <c r="BI2" s="108"/>
-      <c r="BJ2" s="106">
-        <f t="shared" ref="BJ2" si="15">BG2+1</f>
+      <c r="BH2" s="124"/>
+      <c r="BI2" s="125"/>
+      <c r="BJ2" s="123">
+        <f>BG2+1</f>
         <v>20</v>
       </c>
-      <c r="BK2" s="107"/>
-      <c r="BL2" s="108"/>
-      <c r="BM2" s="106">
-        <f t="shared" ref="BM2" si="16">BJ2+1</f>
+      <c r="BK2" s="124"/>
+      <c r="BL2" s="125"/>
+      <c r="BM2" s="123">
+        <f>BJ2+1</f>
         <v>21</v>
       </c>
-      <c r="BN2" s="107"/>
-      <c r="BO2" s="108"/>
-      <c r="BP2" s="106">
-        <f t="shared" ref="BP2" si="17">BM2+1</f>
+      <c r="BN2" s="124"/>
+      <c r="BO2" s="125"/>
+      <c r="BP2" s="123">
+        <f>BM2+1</f>
         <v>22</v>
       </c>
-      <c r="BQ2" s="107"/>
-      <c r="BR2" s="108"/>
-      <c r="BS2" s="106">
-        <f t="shared" ref="BS2" si="18">BP2+1</f>
+      <c r="BQ2" s="124"/>
+      <c r="BR2" s="125"/>
+      <c r="BS2" s="123">
+        <f>BP2+1</f>
         <v>23</v>
       </c>
-      <c r="BT2" s="107"/>
-      <c r="BU2" s="108"/>
-      <c r="BV2" s="106">
+      <c r="BT2" s="124"/>
+      <c r="BU2" s="125"/>
+      <c r="BV2" s="123">
         <f>BS2+1</f>
         <v>24</v>
       </c>
-      <c r="BW2" s="107"/>
-      <c r="BX2" s="108"/>
-      <c r="BY2" s="106">
-        <f t="shared" ref="BY2" si="19">BV2+1</f>
+      <c r="BW2" s="124"/>
+      <c r="BX2" s="125"/>
+      <c r="BY2" s="123">
+        <f>BV2+1</f>
         <v>25</v>
       </c>
-      <c r="BZ2" s="107"/>
-      <c r="CA2" s="108"/>
-      <c r="CB2" s="106">
-        <f t="shared" ref="CB2" si="20">BY2+1</f>
+      <c r="BZ2" s="124"/>
+      <c r="CA2" s="125"/>
+      <c r="CB2" s="123">
+        <f>BY2+1</f>
         <v>26</v>
       </c>
-      <c r="CC2" s="107"/>
-      <c r="CD2" s="108"/>
-      <c r="CE2" s="106">
-        <f t="shared" ref="CE2" si="21">CB2+1</f>
+      <c r="CC2" s="124"/>
+      <c r="CD2" s="125"/>
+      <c r="CE2" s="123">
+        <f>CB2+1</f>
         <v>27</v>
       </c>
-      <c r="CF2" s="107"/>
-      <c r="CG2" s="108"/>
-      <c r="CH2" s="106">
-        <f t="shared" ref="CH2" si="22">CE2+1</f>
+      <c r="CF2" s="124"/>
+      <c r="CG2" s="125"/>
+      <c r="CH2" s="123">
+        <f>CE2+1</f>
         <v>28</v>
       </c>
-      <c r="CI2" s="107"/>
-      <c r="CJ2" s="108"/>
-      <c r="CK2" s="106">
-        <f t="shared" ref="CK2" si="23">CH2+1</f>
+      <c r="CI2" s="124"/>
+      <c r="CJ2" s="125"/>
+      <c r="CK2" s="123">
+        <f>CH2+1</f>
         <v>29</v>
       </c>
-      <c r="CL2" s="107"/>
-      <c r="CM2" s="108"/>
-      <c r="CN2" s="106">
+      <c r="CL2" s="124"/>
+      <c r="CM2" s="125"/>
+      <c r="CN2" s="123">
         <f>CK2+1</f>
         <v>30</v>
       </c>
-      <c r="CO2" s="107"/>
-      <c r="CP2" s="108"/>
-      <c r="CQ2" s="106">
-        <f t="shared" ref="CQ2" si="24">CN2+1</f>
+      <c r="CO2" s="124"/>
+      <c r="CP2" s="125"/>
+      <c r="CQ2" s="123">
+        <f>CN2+1</f>
         <v>31</v>
       </c>
-      <c r="CR2" s="107"/>
-      <c r="CS2" s="108"/>
-      <c r="CT2" s="106">
-        <f t="shared" ref="CT2" si="25">CQ2+1</f>
+      <c r="CR2" s="124"/>
+      <c r="CS2" s="125"/>
+      <c r="CT2" s="123">
+        <f>CQ2+1</f>
         <v>32</v>
       </c>
-      <c r="CU2" s="107"/>
-      <c r="CV2" s="108"/>
-      <c r="CW2" s="106">
-        <f t="shared" ref="CW2" si="26">CT2+1</f>
+      <c r="CU2" s="124"/>
+      <c r="CV2" s="125"/>
+      <c r="CW2" s="123">
+        <f>CT2+1</f>
         <v>33</v>
       </c>
-      <c r="CX2" s="107"/>
-      <c r="CY2" s="108"/>
-      <c r="CZ2" s="106">
-        <f t="shared" ref="CZ2" si="27">CW2+1</f>
+      <c r="CX2" s="124"/>
+      <c r="CY2" s="125"/>
+      <c r="CZ2" s="123">
+        <f>CW2+1</f>
         <v>34</v>
       </c>
-      <c r="DA2" s="107"/>
-      <c r="DB2" s="108"/>
-      <c r="DC2" s="106">
-        <f t="shared" ref="DC2" si="28">CZ2+1</f>
+      <c r="DA2" s="124"/>
+      <c r="DB2" s="125"/>
+      <c r="DC2" s="123">
+        <f>CZ2+1</f>
         <v>35</v>
       </c>
-      <c r="DD2" s="107"/>
-      <c r="DE2" s="108"/>
-      <c r="DF2" s="106">
+      <c r="DD2" s="124"/>
+      <c r="DE2" s="125"/>
+      <c r="DF2" s="123">
         <f>DC2+1</f>
         <v>36</v>
       </c>
-      <c r="DG2" s="107"/>
-      <c r="DH2" s="108"/>
-      <c r="DI2" s="106">
-        <f t="shared" ref="DI2" si="29">DF2+1</f>
+      <c r="DG2" s="124"/>
+      <c r="DH2" s="125"/>
+      <c r="DI2" s="123">
+        <f>DF2+1</f>
         <v>37</v>
       </c>
-      <c r="DJ2" s="107"/>
-      <c r="DK2" s="108"/>
-      <c r="DL2" s="106">
-        <f t="shared" ref="DL2" si="30">DI2+1</f>
+      <c r="DJ2" s="124"/>
+      <c r="DK2" s="125"/>
+      <c r="DL2" s="123">
+        <f>DI2+1</f>
         <v>38</v>
       </c>
-      <c r="DM2" s="107"/>
-      <c r="DN2" s="108"/>
-      <c r="DO2" s="106">
-        <f t="shared" ref="DO2" si="31">DL2+1</f>
+      <c r="DM2" s="124"/>
+      <c r="DN2" s="125"/>
+      <c r="DO2" s="123">
+        <f>DL2+1</f>
         <v>39</v>
       </c>
-      <c r="DP2" s="107"/>
-      <c r="DQ2" s="108"/>
-      <c r="DR2" s="106">
-        <f t="shared" ref="DR2" si="32">DO2+1</f>
+      <c r="DP2" s="124"/>
+      <c r="DQ2" s="125"/>
+      <c r="DR2" s="123">
+        <f>DO2+1</f>
         <v>40</v>
       </c>
-      <c r="DS2" s="107"/>
-      <c r="DT2" s="108"/>
-      <c r="DU2" s="106">
-        <f t="shared" ref="DU2" si="33">DR2+1</f>
+      <c r="DS2" s="124"/>
+      <c r="DT2" s="125"/>
+      <c r="DU2" s="123">
+        <f>DR2+1</f>
         <v>41</v>
       </c>
-      <c r="DV2" s="107"/>
-      <c r="DW2" s="108"/>
-      <c r="DX2" s="106">
+      <c r="DV2" s="124"/>
+      <c r="DW2" s="125"/>
+      <c r="DX2" s="123">
         <f>DU2+1</f>
         <v>42</v>
       </c>
-      <c r="DY2" s="107"/>
-      <c r="DZ2" s="108"/>
-      <c r="EA2" s="106">
-        <f t="shared" ref="EA2" si="34">DX2+1</f>
+      <c r="DY2" s="124"/>
+      <c r="DZ2" s="125"/>
+      <c r="EA2" s="123">
+        <f>DX2+1</f>
         <v>43</v>
       </c>
-      <c r="EB2" s="107"/>
-      <c r="EC2" s="108"/>
-      <c r="ED2" s="106">
-        <f t="shared" ref="ED2" si="35">EA2+1</f>
+      <c r="EB2" s="124"/>
+      <c r="EC2" s="125"/>
+      <c r="ED2" s="123">
+        <f>EA2+1</f>
         <v>44</v>
       </c>
-      <c r="EE2" s="107"/>
-      <c r="EF2" s="108"/>
-      <c r="EG2" s="106">
-        <f t="shared" ref="EG2" si="36">ED2+1</f>
+      <c r="EE2" s="124"/>
+      <c r="EF2" s="125"/>
+      <c r="EG2" s="123">
+        <f>ED2+1</f>
         <v>45</v>
       </c>
-      <c r="EH2" s="107"/>
-      <c r="EI2" s="108"/>
-      <c r="EJ2" s="106">
-        <f t="shared" ref="EJ2" si="37">EG2+1</f>
+      <c r="EH2" s="124"/>
+      <c r="EI2" s="125"/>
+      <c r="EJ2" s="123">
+        <f>EG2+1</f>
         <v>46</v>
       </c>
-      <c r="EK2" s="107"/>
-      <c r="EL2" s="108"/>
-      <c r="EM2" s="106">
-        <f t="shared" ref="EM2" si="38">EJ2+1</f>
+      <c r="EK2" s="124"/>
+      <c r="EL2" s="125"/>
+      <c r="EM2" s="123">
+        <f>EJ2+1</f>
         <v>47</v>
       </c>
-      <c r="EN2" s="107"/>
-      <c r="EO2" s="108"/>
-      <c r="EP2" s="106">
+      <c r="EN2" s="124"/>
+      <c r="EO2" s="125"/>
+      <c r="EP2" s="123">
         <f>EM2+1</f>
         <v>48</v>
       </c>
-      <c r="EQ2" s="107"/>
-      <c r="ER2" s="108"/>
-      <c r="ES2" s="106">
-        <f t="shared" ref="ES2" si="39">EP2+1</f>
+      <c r="EQ2" s="124"/>
+      <c r="ER2" s="125"/>
+      <c r="ES2" s="123">
+        <f>EP2+1</f>
         <v>49</v>
       </c>
-      <c r="ET2" s="107"/>
-      <c r="EU2" s="108"/>
-      <c r="EV2" s="106">
-        <f t="shared" ref="EV2" si="40">ES2+1</f>
+      <c r="ET2" s="124"/>
+      <c r="EU2" s="125"/>
+      <c r="EV2" s="123">
+        <f>ES2+1</f>
         <v>50</v>
       </c>
-      <c r="EW2" s="107"/>
-      <c r="EX2" s="108"/>
-      <c r="EY2" s="106">
-        <f t="shared" ref="EY2" si="41">EV2+1</f>
+      <c r="EW2" s="124"/>
+      <c r="EX2" s="125"/>
+      <c r="EY2" s="123">
+        <f>EV2+1</f>
         <v>51</v>
       </c>
-      <c r="EZ2" s="107"/>
-      <c r="FA2" s="108"/>
-      <c r="FB2" s="106">
-        <f t="shared" ref="FB2" si="42">EY2+1</f>
+      <c r="EZ2" s="124"/>
+      <c r="FA2" s="125"/>
+      <c r="FB2" s="123">
+        <f>EY2+1</f>
         <v>52</v>
       </c>
-      <c r="FC2" s="107"/>
-      <c r="FD2" s="108"/>
+      <c r="FC2" s="124"/>
+      <c r="FD2" s="125"/>
     </row>
     <row r="3" spans="1:160" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="18"/>
@@ -23279,15 +24162,15 @@
         <v>62</v>
       </c>
       <c r="B4" s="26">
-        <f t="shared" ref="B4:D23" si="43">SUMIF($E$3:$FD$3,B$3,$E4:$FD4)</f>
+        <f t="shared" ref="B4:D23" si="0">SUMIF($E$3:$FD$3,B$3,$E4:$FD4)</f>
         <v>0</v>
       </c>
       <c r="C4" s="27">
-        <f t="shared" si="43"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="D4" s="28">
-        <f t="shared" si="43"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E4" s="29">
@@ -23487,15 +24370,15 @@
         <v>7</v>
       </c>
       <c r="B5" s="33">
-        <f t="shared" si="43"/>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="C5" s="34">
-        <f t="shared" si="43"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="D5" s="35">
-        <f t="shared" si="43"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E5" s="36">
@@ -23695,15 +24578,15 @@
         <v>46</v>
       </c>
       <c r="B6" s="33">
-        <f t="shared" si="43"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="C6" s="34">
-        <f t="shared" si="43"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="D6" s="35">
-        <f t="shared" si="43"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E6" s="36">
@@ -23903,15 +24786,15 @@
         <v>8</v>
       </c>
       <c r="B7" s="33">
-        <f t="shared" si="43"/>
+        <f t="shared" si="0"/>
         <v>13</v>
       </c>
       <c r="C7" s="34">
-        <f t="shared" si="43"/>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="D7" s="35">
-        <f t="shared" si="43"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E7" s="36">
@@ -24111,15 +24994,15 @@
         <v>40</v>
       </c>
       <c r="B8" s="33">
-        <f t="shared" si="43"/>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="C8" s="34">
-        <f t="shared" si="43"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="D8" s="35">
-        <f t="shared" si="43"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="E8" s="36">
@@ -24319,15 +25202,15 @@
         <v>26</v>
       </c>
       <c r="B9" s="33">
-        <f t="shared" si="43"/>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="C9" s="34">
-        <f t="shared" si="43"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="D9" s="35">
-        <f t="shared" si="43"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E9" s="36">
@@ -24527,15 +25410,15 @@
         <v>63</v>
       </c>
       <c r="B10" s="33">
-        <f t="shared" si="43"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="C10" s="34">
-        <f t="shared" si="43"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="D10" s="35">
-        <f t="shared" si="43"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E10" s="36">
@@ -24735,15 +25618,15 @@
         <v>64</v>
       </c>
       <c r="B11" s="33">
-        <f t="shared" si="43"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="C11" s="34">
-        <f t="shared" si="43"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="D11" s="35">
-        <f t="shared" si="43"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E11" s="36">
@@ -24943,15 +25826,15 @@
         <v>21</v>
       </c>
       <c r="B12" s="33">
-        <f t="shared" si="43"/>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="C12" s="34">
-        <f t="shared" si="43"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="D12" s="35">
-        <f t="shared" si="43"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E12" s="36">
@@ -25151,15 +26034,15 @@
         <v>15</v>
       </c>
       <c r="B13" s="33">
-        <f t="shared" si="43"/>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="C13" s="34">
-        <f t="shared" si="43"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="D13" s="35">
-        <f t="shared" si="43"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E13" s="36">
@@ -25359,15 +26242,15 @@
         <v>34</v>
       </c>
       <c r="B14" s="33">
-        <f t="shared" si="43"/>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="C14" s="34">
-        <f t="shared" si="43"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="D14" s="35">
-        <f t="shared" si="43"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="E14" s="36">
@@ -25567,15 +26450,15 @@
         <v>65</v>
       </c>
       <c r="B15" s="33">
-        <f t="shared" si="43"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="C15" s="34">
-        <f t="shared" si="43"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="D15" s="35">
-        <f t="shared" si="43"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E15" s="36">
@@ -25775,15 +26658,15 @@
         <v>66</v>
       </c>
       <c r="B16" s="33">
-        <f t="shared" si="43"/>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="C16" s="34">
-        <f t="shared" si="43"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="D16" s="35">
-        <f t="shared" si="43"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E16" s="36">
@@ -25983,15 +26866,15 @@
         <v>28</v>
       </c>
       <c r="B17" s="33">
-        <f t="shared" si="43"/>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="C17" s="34">
-        <f t="shared" si="43"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="D17" s="35">
-        <f t="shared" si="43"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E17" s="36">
@@ -26191,15 +27074,15 @@
         <v>24</v>
       </c>
       <c r="B18" s="33">
-        <f t="shared" si="43"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="C18" s="34">
-        <f t="shared" si="43"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="D18" s="35">
-        <f t="shared" si="43"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E18" s="36">
@@ -26399,15 +27282,15 @@
         <v>37</v>
       </c>
       <c r="B19" s="33">
-        <f t="shared" si="43"/>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="C19" s="34">
-        <f t="shared" si="43"/>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="D19" s="35">
-        <f t="shared" si="43"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E19" s="36">
@@ -26607,15 +27490,15 @@
         <v>19</v>
       </c>
       <c r="B20" s="33">
-        <f t="shared" si="43"/>
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="C20" s="34">
-        <f t="shared" si="43"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="D20" s="35">
-        <f t="shared" si="43"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E20" s="36">
@@ -26815,15 +27698,15 @@
         <v>67</v>
       </c>
       <c r="B21" s="33">
-        <f t="shared" si="43"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="C21" s="34">
-        <f t="shared" si="43"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="D21" s="35">
-        <f t="shared" si="43"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E21" s="36">
@@ -27023,15 +27906,15 @@
         <v>45</v>
       </c>
       <c r="B22" s="33">
-        <f t="shared" si="43"/>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="C22" s="34">
-        <f t="shared" si="43"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="D22" s="35">
-        <f t="shared" si="43"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E22" s="36">
@@ -27231,15 +28114,15 @@
         <v>68</v>
       </c>
       <c r="B23" s="33">
-        <f t="shared" si="43"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="C23" s="34">
-        <f t="shared" si="43"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="D23" s="35">
-        <f t="shared" si="43"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E23" s="36">
@@ -27439,15 +28322,15 @@
         <v>69</v>
       </c>
       <c r="B24" s="33">
-        <f t="shared" ref="B24:D43" si="44">SUMIF($E$3:$FD$3,B$3,$E24:$FD24)</f>
+        <f t="shared" ref="B24:D43" si="1">SUMIF($E$3:$FD$3,B$3,$E24:$FD24)</f>
         <v>0</v>
       </c>
       <c r="C24" s="34">
-        <f t="shared" si="44"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="D24" s="35">
-        <f t="shared" si="44"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="E24" s="36">
@@ -27647,15 +28530,15 @@
         <v>36</v>
       </c>
       <c r="B25" s="33">
-        <f t="shared" si="44"/>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="C25" s="34">
-        <f t="shared" si="44"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="D25" s="35">
-        <f t="shared" si="44"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="E25" s="36">
@@ -27855,15 +28738,15 @@
         <v>70</v>
       </c>
       <c r="B26" s="33">
-        <f t="shared" si="44"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="C26" s="34">
-        <f t="shared" si="44"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="D26" s="35">
-        <f t="shared" si="44"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="E26" s="36">
@@ -28063,15 +28946,15 @@
         <v>5</v>
       </c>
       <c r="B27" s="33">
-        <f t="shared" si="44"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="C27" s="34">
-        <f t="shared" si="44"/>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="D27" s="35">
-        <f t="shared" si="44"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="E27" s="36">
@@ -28271,15 +29154,15 @@
         <v>33</v>
       </c>
       <c r="B28" s="33">
-        <f t="shared" si="44"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="C28" s="34">
-        <f t="shared" si="44"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="D28" s="35">
-        <f t="shared" si="44"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="E28" s="36">
@@ -28479,15 +29362,15 @@
         <v>12</v>
       </c>
       <c r="B29" s="33">
-        <f t="shared" si="44"/>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="C29" s="34">
-        <f t="shared" si="44"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="D29" s="35">
-        <f t="shared" si="44"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="E29" s="36">
@@ -28687,15 +29570,15 @@
         <v>71</v>
       </c>
       <c r="B30" s="33">
-        <f t="shared" si="44"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="C30" s="34">
-        <f t="shared" si="44"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="D30" s="35">
-        <f t="shared" si="44"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="E30" s="36">
@@ -28895,15 +29778,15 @@
         <v>72</v>
       </c>
       <c r="B31" s="33">
-        <f t="shared" si="44"/>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="C31" s="34">
-        <f t="shared" si="44"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="D31" s="35">
-        <f t="shared" si="44"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="E31" s="36">
@@ -29103,15 +29986,15 @@
         <v>18</v>
       </c>
       <c r="B32" s="33">
-        <f t="shared" si="44"/>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="C32" s="34">
-        <f t="shared" si="44"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="D32" s="35">
-        <f t="shared" si="44"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="E32" s="36">
@@ -29311,15 +30194,15 @@
         <v>4</v>
       </c>
       <c r="B33" s="33">
-        <f t="shared" si="44"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="C33" s="34">
-        <f t="shared" si="44"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="D33" s="35">
-        <f t="shared" si="44"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="E33" s="36">
@@ -29519,15 +30402,15 @@
         <v>73</v>
       </c>
       <c r="B34" s="33">
-        <f t="shared" si="44"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="C34" s="34">
-        <f t="shared" si="44"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="D34" s="35">
-        <f t="shared" si="44"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="E34" s="36">
@@ -29727,15 +30610,15 @@
         <v>74</v>
       </c>
       <c r="B35" s="33">
-        <f t="shared" si="44"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="C35" s="34">
-        <f t="shared" si="44"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="D35" s="35">
-        <f t="shared" si="44"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="E35" s="36">
@@ -29935,15 +30818,15 @@
         <v>75</v>
       </c>
       <c r="B36" s="33">
-        <f t="shared" si="44"/>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="C36" s="34">
-        <f t="shared" si="44"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="D36" s="35">
-        <f t="shared" si="44"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="E36" s="36">
@@ -30143,15 +31026,15 @@
         <v>13</v>
       </c>
       <c r="B37" s="33">
-        <f t="shared" si="44"/>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="C37" s="34">
-        <f t="shared" si="44"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="D37" s="35">
-        <f t="shared" si="44"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="E37" s="36">
@@ -30351,15 +31234,15 @@
         <v>29</v>
       </c>
       <c r="B38" s="33">
-        <f t="shared" si="44"/>
+        <f t="shared" si="1"/>
         <v>7</v>
       </c>
       <c r="C38" s="34">
-        <f t="shared" si="44"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="D38" s="35">
-        <f t="shared" si="44"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="E38" s="36">
@@ -30559,15 +31442,15 @@
         <v>39</v>
       </c>
       <c r="B39" s="33">
-        <f t="shared" si="44"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="C39" s="34">
-        <f t="shared" si="44"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="D39" s="35">
-        <f t="shared" si="44"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="E39" s="36">
@@ -30767,15 +31650,15 @@
         <v>30</v>
       </c>
       <c r="B40" s="33">
-        <f t="shared" si="44"/>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="C40" s="34">
-        <f t="shared" si="44"/>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="D40" s="35">
-        <f t="shared" si="44"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="E40" s="36">
@@ -30975,15 +31858,15 @@
         <v>17</v>
       </c>
       <c r="B41" s="33">
-        <f t="shared" si="44"/>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="C41" s="34">
-        <f t="shared" si="44"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="D41" s="35">
-        <f t="shared" si="44"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="E41" s="36">
@@ -31183,15 +32066,15 @@
         <v>23</v>
       </c>
       <c r="B42" s="33">
-        <f t="shared" si="44"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="C42" s="34">
-        <f t="shared" si="44"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="D42" s="35">
-        <f t="shared" si="44"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="E42" s="36">
@@ -31391,15 +32274,15 @@
         <v>48</v>
       </c>
       <c r="B43" s="33">
-        <f t="shared" si="44"/>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="C43" s="34">
-        <f t="shared" si="44"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="D43" s="35">
-        <f t="shared" si="44"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="E43" s="36">
@@ -31599,15 +32482,15 @@
         <v>10</v>
       </c>
       <c r="B44" s="33">
-        <f t="shared" ref="B44:D62" si="45">SUMIF($E$3:$FD$3,B$3,$E44:$FD44)</f>
+        <f t="shared" ref="B44:D62" si="2">SUMIF($E$3:$FD$3,B$3,$E44:$FD44)</f>
         <v>1</v>
       </c>
       <c r="C44" s="34">
-        <f t="shared" si="45"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="D44" s="35">
-        <f t="shared" si="45"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="E44" s="36">
@@ -31807,15 +32690,15 @@
         <v>76</v>
       </c>
       <c r="B45" s="33">
-        <f t="shared" si="45"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="C45" s="34">
-        <f t="shared" si="45"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="D45" s="35">
-        <f t="shared" si="45"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="E45" s="36">
@@ -32015,15 +32898,15 @@
         <v>14</v>
       </c>
       <c r="B46" s="33">
-        <f t="shared" si="45"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="C46" s="34">
-        <f t="shared" si="45"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="D46" s="35">
-        <f t="shared" si="45"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="E46" s="36">
@@ -32223,15 +33106,15 @@
         <v>6</v>
       </c>
       <c r="B47" s="33">
-        <f t="shared" si="45"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="C47" s="34">
-        <f t="shared" si="45"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="D47" s="35">
-        <f t="shared" si="45"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="E47" s="36">
@@ -32431,15 +33314,15 @@
         <v>49</v>
       </c>
       <c r="B48" s="33">
-        <f t="shared" si="45"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="C48" s="34">
-        <f t="shared" si="45"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="D48" s="35">
-        <f t="shared" si="45"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="E48" s="36">
@@ -32639,15 +33522,15 @@
         <v>22</v>
       </c>
       <c r="B49" s="33">
-        <f t="shared" si="45"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="C49" s="34">
-        <f t="shared" si="45"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="D49" s="35">
-        <f t="shared" si="45"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="E49" s="36">
@@ -32847,15 +33730,15 @@
         <v>11</v>
       </c>
       <c r="B50" s="33">
-        <f t="shared" si="45"/>
+        <f t="shared" si="2"/>
         <v>5</v>
       </c>
       <c r="C50" s="34">
-        <f t="shared" si="45"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="D50" s="35">
-        <f t="shared" si="45"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="E50" s="36">
@@ -33055,15 +33938,15 @@
         <v>77</v>
       </c>
       <c r="B51" s="33">
-        <f t="shared" si="45"/>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="C51" s="34">
-        <f t="shared" si="45"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="D51" s="35">
-        <f t="shared" si="45"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="E51" s="36">
@@ -33263,15 +34146,15 @@
         <v>78</v>
       </c>
       <c r="B52" s="33">
-        <f t="shared" si="45"/>
+        <f t="shared" si="2"/>
         <v>5</v>
       </c>
       <c r="C52" s="34">
-        <f t="shared" si="45"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="D52" s="35">
-        <f t="shared" si="45"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="E52" s="36">
@@ -33471,15 +34354,15 @@
         <v>79</v>
       </c>
       <c r="B53" s="33">
-        <f t="shared" si="45"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="C53" s="34">
-        <f t="shared" si="45"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="D53" s="35">
-        <f t="shared" si="45"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="E53" s="36">
@@ -33679,15 +34562,15 @@
         <v>16</v>
       </c>
       <c r="B54" s="33">
-        <f t="shared" si="45"/>
+        <f t="shared" si="2"/>
         <v>20</v>
       </c>
       <c r="C54" s="34">
-        <f t="shared" si="45"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="D54" s="35">
-        <f t="shared" si="45"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="E54" s="36">
@@ -33887,15 +34770,15 @@
         <v>38</v>
       </c>
       <c r="B55" s="33">
-        <f t="shared" si="45"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="C55" s="34">
-        <f t="shared" si="45"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="D55" s="35">
-        <f t="shared" si="45"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="E55" s="36">
@@ -34095,15 +34978,15 @@
         <v>47</v>
       </c>
       <c r="B56" s="33">
-        <f t="shared" si="45"/>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="C56" s="34">
-        <f t="shared" si="45"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="D56" s="35">
-        <f t="shared" si="45"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="E56" s="36">
@@ -34303,15 +35186,15 @@
         <v>32</v>
       </c>
       <c r="B57" s="33">
-        <f t="shared" si="45"/>
+        <f t="shared" si="2"/>
         <v>9</v>
       </c>
       <c r="C57" s="34">
-        <f t="shared" si="45"/>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="D57" s="35">
-        <f t="shared" si="45"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="E57" s="36">
@@ -34511,15 +35394,15 @@
         <v>35</v>
       </c>
       <c r="B58" s="33">
-        <f t="shared" si="45"/>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="C58" s="34">
-        <f t="shared" si="45"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="D58" s="35">
-        <f t="shared" si="45"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="E58" s="36">
@@ -34719,15 +35602,15 @@
         <v>9</v>
       </c>
       <c r="B59" s="33">
-        <f t="shared" si="45"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="C59" s="34">
-        <f t="shared" si="45"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="D59" s="35">
-        <f t="shared" si="45"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="E59" s="36">
@@ -34927,15 +35810,15 @@
         <v>25</v>
       </c>
       <c r="B60" s="33">
-        <f t="shared" si="45"/>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="C60" s="34">
-        <f t="shared" si="45"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="D60" s="35">
-        <f t="shared" si="45"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="E60" s="36">
@@ -35135,15 +36018,15 @@
         <v>44</v>
       </c>
       <c r="B61" s="33">
-        <f t="shared" si="45"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="C61" s="34">
-        <f t="shared" si="45"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="D61" s="35">
-        <f t="shared" si="45"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="E61" s="36">
@@ -35343,15 +36226,15 @@
         <v>31</v>
       </c>
       <c r="B62" s="40">
-        <f t="shared" si="45"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="C62" s="41">
-        <f t="shared" si="45"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="D62" s="42">
-        <f t="shared" si="45"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="E62" s="43">
@@ -35548,39 +36431,39 @@
     </row>
     <row r="63" spans="1:160" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="Q63" s="49">
-        <f>SUM(Q4:Q62)</f>
+        <f t="shared" ref="Q63:Y63" si="3">SUM(Q4:Q62)</f>
         <v>34</v>
       </c>
       <c r="R63" s="50">
-        <f t="shared" ref="R63:S63" si="46">SUM(R4:R62)</f>
+        <f t="shared" si="3"/>
         <v>28</v>
       </c>
       <c r="S63" s="51">
-        <f t="shared" si="46"/>
+        <f t="shared" si="3"/>
         <v>8</v>
       </c>
       <c r="T63" s="49">
-        <f>SUM(T4:T62)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="U63" s="50">
-        <f t="shared" ref="U63:V63" si="47">SUM(U4:U62)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="V63" s="51">
-        <f t="shared" si="47"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="W63" s="49">
-        <f>SUM(W4:W62)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="X63" s="50">
-        <f t="shared" ref="X63:Y63" si="48">SUM(X4:X62)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="Y63" s="51">
-        <f t="shared" si="48"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>

</xml_diff>